<commit_message>
Eliminado el documento de cambios
</commit_message>
<xml_diff>
--- a/Procesos/ControlDeCambios/Plantillas.xlsx
+++ b/Procesos/ControlDeCambios/Plantillas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/roi_martinez_enriquez_rai_usc_es/Documents/GrEI/EnSo/6_GestConf/Semana1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/roi_martinez_enriquez_rai_usc_es/Documents/GrEI/EnSo/6_GestConf/Semana2/Arquivos/Documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1156" documentId="8_{510C91CE-A6A1-4AC1-8291-D918ED7F11D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{675F6B9B-F706-4BC5-AB4D-31FB2AAA1760}"/>
+  <xr:revisionPtr revIDLastSave="1231" documentId="8_{510C91CE-A6A1-4AC1-8291-D918ED7F11D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F18E18A-5F73-49EB-BC74-5A7E2FD4F56B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6645DB64-4FE3-44F8-AF56-BC889C6C1641}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="7" xr2:uid="{6645DB64-4FE3-44F8-AF56-BC889C6C1641}"/>
   </bookViews>
   <sheets>
     <sheet name="IdfSlc" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Pruebas" sheetId="6" r:id="rId6"/>
     <sheet name="Revisión" sheetId="9" r:id="rId7"/>
     <sheet name="Cierre" sheetId="8" r:id="rId8"/>
+    <sheet name="Rechazo" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="145">
   <si>
     <t xml:space="preserve">ID: </t>
   </si>
@@ -412,12 +413,6 @@
     <t>[Detalles de los aspectos revisados y evaluados]</t>
   </si>
   <si>
-    <t xml:space="preserve">   Correcciones Implementadas: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Número de corrección]: [Descripción detallada de la corrección] </t>
-  </si>
-  <si>
     <t>Conclusiones</t>
   </si>
   <si>
@@ -430,7 +425,7 @@
     <t>Cierr_001</t>
   </si>
   <si>
-    <t>Responsable del proyecto</t>
+    <t>Responsable del cierre</t>
   </si>
   <si>
     <t xml:space="preserve"> [Nombre completo del responsable]</t>
@@ -439,7 +434,7 @@
     <t>[Número de empleado asignado al responsable]</t>
   </si>
   <si>
-    <t>Resumen del proyecto</t>
+    <t>Resumen del cambio</t>
   </si>
   <si>
     <t>Objetivos iniciales</t>
@@ -454,18 +449,23 @@
     <t>[Lista de cambios realizados]</t>
   </si>
   <si>
-    <t>Evaluación del proyecto</t>
+    <t>Evaluación del cambio</t>
   </si>
   <si>
     <r>
-      <t>Éxito del proyecto</t>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Éxito del cambio</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="1"/>
       </rPr>
       <t>:</t>
     </r>
@@ -477,16 +477,43 @@
     <t>Aspectos destacados</t>
   </si>
   <si>
-    <t xml:space="preserve">[Logros y aspectos positivos del proyecto] </t>
+    <t xml:space="preserve">[Logros y aspectos positivos del cambio] </t>
   </si>
   <si>
     <t>CIERRE</t>
   </si>
   <si>
-    <t>Urgencia (valor):</t>
-  </si>
-  <si>
-    <t>[Indique el nivel de urgencia del cambio solicitado: 1,3,5,10]</t>
+    <t>Rechazo_001</t>
+  </si>
+  <si>
+    <t>EvalDes_001 Ó EvalCCB_001</t>
+  </si>
+  <si>
+    <t>Responsable de la comunicación</t>
+  </si>
+  <si>
+    <t>Resolución</t>
+  </si>
+  <si>
+    <t>Fecha de la decisión:</t>
+  </si>
+  <si>
+    <t>[dd/mm/aa]</t>
+  </si>
+  <si>
+    <t>Responsable:</t>
+  </si>
+  <si>
+    <t>[Desarrollador (Nombre + ID + Correo); o CCB]</t>
+  </si>
+  <si>
+    <t>Justificación:</t>
+  </si>
+  <si>
+    <t>[Se proporcionan detalles para el cliente sobre las razones específicas por las cuales el cambio propuesto ha sido rechazado]</t>
+  </si>
+  <si>
+    <t>NOTIFICACION DE RECHAZO</t>
   </si>
 </sst>
 </file>
@@ -610,12 +637,6 @@
       <name val="Calibri Light"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -651,11 +672,15 @@
       <name val="WordVisi_MSFontService"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
+      <i/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri Light"/>
-      <scheme val="major"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="5">
@@ -684,7 +709,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="82">
+  <borders count="84">
     <border>
       <left/>
       <right/>
@@ -1599,11 +1624,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="246">
+  <cellXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
@@ -1718,19 +1765,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1765,7 +1806,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1781,10 +1821,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1805,6 +1842,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2024,10 +2070,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2060,7 +2103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2123,10 +2166,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2153,7 +2196,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2171,7 +2214,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2186,35 +2229,35 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="82" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2234,7 +2277,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2532,11 +2575,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115ECF1D-1941-4B15-9C92-5FF7A18278F1}">
   <dimension ref="C2:P35"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J8" sqref="C4:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="3:10" ht="15.75" thickBot="1"/>
     <row r="3" spans="3:10" ht="15.75" thickBot="1">
@@ -2558,10 +2601,10 @@
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="3:10">
-      <c r="C4" s="113" t="s">
+      <c r="C4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="114"/>
+      <c r="D4" s="113"/>
       <c r="J4" s="14"/>
     </row>
     <row r="5" spans="3:10">
@@ -2569,31 +2612,31 @@
       <c r="J5" s="14"/>
     </row>
     <row r="6" spans="3:10">
-      <c r="C6" s="115" t="s">
+      <c r="C6" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="126" t="s">
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="126" t="s">
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="3:10">
@@ -2607,10 +2650,10 @@
       <c r="J8" s="17"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="114"/>
+      <c r="D9" s="113"/>
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="3:10">
@@ -2618,108 +2661,108 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="3:10">
-      <c r="C11" s="115" t="s">
+      <c r="C11" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="115"/>
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="3:10">
       <c r="C12" s="13"/>
-      <c r="D12" s="117" t="s">
+      <c r="D12" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="118"/>
-      <c r="J12" s="119"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="117"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="117"/>
+      <c r="I12" s="117"/>
+      <c r="J12" s="118"/>
     </row>
     <row r="13" spans="3:10">
       <c r="C13" s="13"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="121"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="121"/>
-      <c r="H13" s="121"/>
-      <c r="I13" s="121"/>
-      <c r="J13" s="122"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="120"/>
+      <c r="I13" s="120"/>
+      <c r="J13" s="121"/>
     </row>
     <row r="14" spans="3:10">
       <c r="C14" s="13"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="124"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="124"/>
-      <c r="H14" s="124"/>
-      <c r="I14" s="124"/>
-      <c r="J14" s="125"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="123"/>
+      <c r="I14" s="123"/>
+      <c r="J14" s="124"/>
     </row>
     <row r="15" spans="3:10">
       <c r="C15" s="13"/>
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="3:10">
-      <c r="C16" s="115" t="s">
+      <c r="C16" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="115"/>
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="3:16">
       <c r="C17" s="13"/>
-      <c r="D17" s="117" t="s">
+      <c r="D17" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="119"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="117"/>
+      <c r="I17" s="117"/>
+      <c r="J17" s="118"/>
     </row>
     <row r="18" spans="3:16">
       <c r="C18" s="13"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="121"/>
-      <c r="F18" s="121"/>
-      <c r="G18" s="121"/>
-      <c r="H18" s="121"/>
-      <c r="I18" s="121"/>
-      <c r="J18" s="122"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="120"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="121"/>
     </row>
     <row r="19" spans="3:16">
       <c r="C19" s="13"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="121"/>
-      <c r="F19" s="121"/>
-      <c r="G19" s="121"/>
-      <c r="H19" s="121"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="122"/>
+      <c r="D19" s="119"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="121"/>
     </row>
     <row r="20" spans="3:16">
       <c r="C20" s="13"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="121"/>
-      <c r="F20" s="121"/>
-      <c r="G20" s="121"/>
-      <c r="H20" s="121"/>
-      <c r="I20" s="121"/>
-      <c r="J20" s="122"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="120"/>
+      <c r="F20" s="120"/>
+      <c r="G20" s="120"/>
+      <c r="H20" s="120"/>
+      <c r="I20" s="120"/>
+      <c r="J20" s="121"/>
     </row>
     <row r="21" spans="3:16">
       <c r="C21" s="13"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="124"/>
-      <c r="F21" s="124"/>
-      <c r="G21" s="124"/>
-      <c r="H21" s="124"/>
-      <c r="I21" s="124"/>
-      <c r="J21" s="125"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="123"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="123"/>
+      <c r="I21" s="123"/>
+      <c r="J21" s="124"/>
     </row>
     <row r="22" spans="3:16">
       <c r="C22" s="16"/>
@@ -2732,10 +2775,10 @@
       <c r="J22" s="17"/>
     </row>
     <row r="23" spans="3:16">
-      <c r="C23" s="113" t="s">
+      <c r="C23" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="114"/>
+      <c r="D23" s="113"/>
       <c r="J23" s="14"/>
     </row>
     <row r="24" spans="3:16">
@@ -2743,89 +2786,89 @@
       <c r="J24" s="14"/>
     </row>
     <row r="25" spans="3:16">
-      <c r="C25" s="115" t="s">
+      <c r="C25" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="116"/>
-      <c r="E25" s="116"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="115"/>
       <c r="J25" s="14"/>
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="3:16">
       <c r="C26" s="13"/>
-      <c r="D26" s="117" t="s">
+      <c r="D26" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="118"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="118"/>
-      <c r="J26" s="119"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="117"/>
+      <c r="H26" s="117"/>
+      <c r="I26" s="117"/>
+      <c r="J26" s="118"/>
     </row>
     <row r="27" spans="3:16">
       <c r="C27" s="13"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="121"/>
-      <c r="F27" s="121"/>
-      <c r="G27" s="121"/>
-      <c r="H27" s="121"/>
-      <c r="I27" s="121"/>
-      <c r="J27" s="122"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="120"/>
+      <c r="G27" s="120"/>
+      <c r="H27" s="120"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="121"/>
     </row>
     <row r="28" spans="3:16">
       <c r="C28" s="13"/>
-      <c r="D28" s="123"/>
-      <c r="E28" s="124"/>
-      <c r="F28" s="124"/>
-      <c r="G28" s="124"/>
-      <c r="H28" s="124"/>
-      <c r="I28" s="124"/>
-      <c r="J28" s="125"/>
+      <c r="D28" s="122"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="123"/>
+      <c r="G28" s="123"/>
+      <c r="H28" s="123"/>
+      <c r="I28" s="123"/>
+      <c r="J28" s="124"/>
     </row>
     <row r="29" spans="3:16">
       <c r="C29" s="13"/>
       <c r="J29" s="14"/>
     </row>
     <row r="30" spans="3:16">
-      <c r="C30" s="115" t="s">
+      <c r="C30" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="116"/>
-      <c r="E30" s="116"/>
+      <c r="D30" s="115"/>
+      <c r="E30" s="115"/>
       <c r="J30" s="14"/>
     </row>
     <row r="31" spans="3:16">
       <c r="C31" s="13"/>
-      <c r="D31" s="117" t="s">
+      <c r="D31" s="116" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="118"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="118"/>
-      <c r="J31" s="119"/>
+      <c r="E31" s="117"/>
+      <c r="F31" s="117"/>
+      <c r="G31" s="117"/>
+      <c r="H31" s="117"/>
+      <c r="I31" s="117"/>
+      <c r="J31" s="118"/>
     </row>
     <row r="32" spans="3:16">
       <c r="C32" s="13"/>
-      <c r="D32" s="120"/>
-      <c r="E32" s="121"/>
-      <c r="F32" s="121"/>
-      <c r="G32" s="121"/>
-      <c r="H32" s="121"/>
-      <c r="I32" s="121"/>
-      <c r="J32" s="122"/>
+      <c r="D32" s="119"/>
+      <c r="E32" s="120"/>
+      <c r="F32" s="120"/>
+      <c r="G32" s="120"/>
+      <c r="H32" s="120"/>
+      <c r="I32" s="120"/>
+      <c r="J32" s="121"/>
     </row>
     <row r="33" spans="3:10">
       <c r="C33" s="13"/>
-      <c r="D33" s="123"/>
-      <c r="E33" s="124"/>
-      <c r="F33" s="124"/>
-      <c r="G33" s="124"/>
-      <c r="H33" s="124"/>
-      <c r="I33" s="124"/>
-      <c r="J33" s="125"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="123"/>
+      <c r="F33" s="123"/>
+      <c r="G33" s="123"/>
+      <c r="H33" s="123"/>
+      <c r="I33" s="123"/>
+      <c r="J33" s="124"/>
     </row>
     <row r="34" spans="3:10" ht="15.75" thickBot="1">
       <c r="C34" s="18"/>
@@ -2838,18 +2881,18 @@
       <c r="J34" s="20"/>
     </row>
     <row r="35" spans="3:10" ht="15.75" thickBot="1">
-      <c r="C35" s="109" t="s">
+      <c r="C35" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="110"/>
-      <c r="E35" s="110"/>
-      <c r="F35" s="110"/>
-      <c r="G35" s="110"/>
-      <c r="H35" s="110"/>
-      <c r="I35" s="111" t="s">
+      <c r="D35" s="109"/>
+      <c r="E35" s="109"/>
+      <c r="F35" s="109"/>
+      <c r="G35" s="109"/>
+      <c r="H35" s="109"/>
+      <c r="I35" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="112"/>
+      <c r="J35" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -2878,13 +2921,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7651F806-68F4-4E68-A906-F21ED235D482}">
-  <dimension ref="C2:P35"/>
+  <dimension ref="C2:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="3:13" ht="15.75" thickBot="1"/>
     <row r="3" spans="3:13">
@@ -2906,24 +2949,24 @@
       <c r="J3" s="30"/>
     </row>
     <row r="4" spans="3:13">
-      <c r="C4" s="136" t="s">
+      <c r="C4" s="135" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="138" t="s">
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="139"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="138"/>
     </row>
     <row r="5" spans="3:13">
-      <c r="C5" s="113" t="s">
+      <c r="C5" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="114"/>
+      <c r="D5" s="113"/>
       <c r="J5" s="14"/>
     </row>
     <row r="6" spans="3:13">
@@ -2931,45 +2974,45 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="3:13">
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="126" t="s">
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="3:13">
-      <c r="C8" s="115" t="s">
+      <c r="C8" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="126" t="s">
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="3:13">
-      <c r="C9" s="115" t="s">
+      <c r="C9" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="126" t="s">
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="126"/>
-      <c r="H9" s="126"/>
-      <c r="I9" s="126"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="125"/>
+      <c r="I9" s="125"/>
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="3:13" ht="15.75">
@@ -2984,10 +3027,10 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="3:13">
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="113"/>
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="3:13">
@@ -2995,55 +3038,55 @@
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="3:13">
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="3:13">
       <c r="C14" s="13"/>
-      <c r="D14" s="127" t="s">
+      <c r="D14" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="128"/>
-      <c r="F14" s="128"/>
-      <c r="G14" s="128"/>
-      <c r="H14" s="128"/>
-      <c r="I14" s="128"/>
-      <c r="J14" s="129"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="128"/>
     </row>
     <row r="15" spans="3:13">
       <c r="C15" s="13"/>
-      <c r="D15" s="130"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="131"/>
-      <c r="G15" s="131"/>
-      <c r="H15" s="131"/>
-      <c r="I15" s="131"/>
-      <c r="J15" s="132"/>
+      <c r="D15" s="129"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="131"/>
     </row>
     <row r="16" spans="3:13">
       <c r="C16" s="13"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="134"/>
-      <c r="F16" s="134"/>
-      <c r="G16" s="134"/>
-      <c r="H16" s="134"/>
-      <c r="I16" s="134"/>
-      <c r="J16" s="135"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="133"/>
+      <c r="I16" s="133"/>
+      <c r="J16" s="134"/>
     </row>
     <row r="17" spans="3:16">
       <c r="C17" s="13"/>
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="3:16">
-      <c r="C18" s="115" t="s">
+      <c r="C18" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="116"/>
-      <c r="E18" s="116"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="115"/>
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="3:16">
@@ -3063,11 +3106,11 @@
       <c r="J20" s="14"/>
     </row>
     <row r="21" spans="3:16">
-      <c r="C21" s="115" t="s">
+      <c r="C21" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="116"/>
-      <c r="E21" s="116"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115"/>
       <c r="J21" s="14"/>
     </row>
     <row r="22" spans="3:16">
@@ -3102,116 +3145,82 @@
       <c r="J25" s="14"/>
     </row>
     <row r="26" spans="3:16">
-      <c r="C26" s="115" t="s">
+      <c r="C26" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="116"/>
-      <c r="E26" s="116"/>
+      <c r="D26" s="115"/>
+      <c r="E26" s="115"/>
       <c r="J26" s="14"/>
     </row>
     <row r="27" spans="3:16">
       <c r="C27" s="13"/>
-      <c r="D27" s="127" t="s">
+      <c r="D27" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="128"/>
-      <c r="F27" s="128"/>
-      <c r="G27" s="128"/>
-      <c r="H27" s="128"/>
-      <c r="I27" s="128"/>
-      <c r="J27" s="129"/>
+      <c r="E27" s="127"/>
+      <c r="F27" s="127"/>
+      <c r="G27" s="127"/>
+      <c r="H27" s="127"/>
+      <c r="I27" s="127"/>
+      <c r="J27" s="128"/>
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="3:16">
       <c r="C28" s="13"/>
-      <c r="D28" s="130"/>
-      <c r="E28" s="131"/>
-      <c r="F28" s="131"/>
-      <c r="G28" s="131"/>
-      <c r="H28" s="131"/>
-      <c r="I28" s="131"/>
-      <c r="J28" s="132"/>
+      <c r="D28" s="129"/>
+      <c r="E28" s="130"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="130"/>
+      <c r="J28" s="131"/>
     </row>
     <row r="29" spans="3:16">
       <c r="C29" s="13"/>
-      <c r="D29" s="130"/>
-      <c r="E29" s="131"/>
-      <c r="F29" s="131"/>
-      <c r="G29" s="131"/>
-      <c r="H29" s="131"/>
-      <c r="I29" s="131"/>
-      <c r="J29" s="132"/>
+      <c r="D29" s="129"/>
+      <c r="E29" s="130"/>
+      <c r="F29" s="130"/>
+      <c r="G29" s="130"/>
+      <c r="H29" s="130"/>
+      <c r="I29" s="130"/>
+      <c r="J29" s="131"/>
     </row>
     <row r="30" spans="3:16">
       <c r="C30" s="13"/>
-      <c r="D30" s="133"/>
-      <c r="E30" s="134"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="134"/>
-      <c r="I30" s="134"/>
-      <c r="J30" s="135"/>
-    </row>
-    <row r="31" spans="3:16">
-      <c r="C31" s="13"/>
-      <c r="D31" s="241"/>
-      <c r="E31" s="241"/>
-      <c r="F31" s="241"/>
-      <c r="G31" s="241"/>
-      <c r="H31" s="241"/>
-      <c r="I31" s="241"/>
-      <c r="J31" s="108"/>
-    </row>
-    <row r="32" spans="3:16">
-      <c r="C32" s="115" t="s">
-        <v>136</v>
-      </c>
-      <c r="D32" s="242"/>
-      <c r="E32" s="242"/>
-      <c r="F32" s="241"/>
-      <c r="G32" s="241"/>
-      <c r="H32" s="241"/>
-      <c r="I32" s="241"/>
-      <c r="J32" s="108"/>
-    </row>
-    <row r="33" spans="3:10">
-      <c r="C33" s="13"/>
-      <c r="D33" s="243" t="s">
-        <v>137</v>
-      </c>
-      <c r="E33" s="244"/>
-      <c r="F33" s="244"/>
-      <c r="G33" s="244"/>
-      <c r="H33" s="244"/>
-      <c r="I33" s="244"/>
-      <c r="J33" s="245"/>
-    </row>
-    <row r="34" spans="3:10" ht="15.75" thickBot="1">
-      <c r="C34" s="18"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="20"/>
-    </row>
-    <row r="35" spans="3:10" ht="15.75" thickBot="1">
-      <c r="C35" s="109" t="s">
+      <c r="D30" s="132"/>
+      <c r="E30" s="133"/>
+      <c r="F30" s="133"/>
+      <c r="G30" s="133"/>
+      <c r="H30" s="133"/>
+      <c r="I30" s="133"/>
+      <c r="J30" s="134"/>
+    </row>
+    <row r="31" spans="3:16" ht="15.75" thickBot="1">
+      <c r="C31" s="18"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="20"/>
+    </row>
+    <row r="32" spans="3:16" ht="15.75" thickBot="1">
+      <c r="C32" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="110"/>
-      <c r="E35" s="110"/>
-      <c r="F35" s="110"/>
-      <c r="G35" s="110"/>
-      <c r="H35" s="110"/>
-      <c r="I35" s="111" t="s">
+      <c r="D32" s="109"/>
+      <c r="E32" s="109"/>
+      <c r="F32" s="109"/>
+      <c r="G32" s="109"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="112"/>
+      <c r="J32" s="111"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="18">
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="C8:E8"/>
@@ -3224,14 +3233,12 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I32:J32"/>
     <mergeCell ref="D27:J30"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="C32:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3246,7 +3253,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="3:13" ht="15.75" thickBot="1"/>
     <row r="3" spans="3:13">
@@ -3268,24 +3275,24 @@
       <c r="J3" s="30"/>
     </row>
     <row r="4" spans="3:13">
-      <c r="C4" s="136" t="s">
+      <c r="C4" s="135" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="138" t="s">
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="139"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="138"/>
     </row>
     <row r="5" spans="3:13">
-      <c r="C5" s="113" t="s">
+      <c r="C5" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="114"/>
+      <c r="D5" s="113"/>
       <c r="J5" s="14"/>
     </row>
     <row r="6" spans="3:13">
@@ -3293,59 +3300,59 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="3:13">
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="126" t="s">
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="125" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="3:13">
-      <c r="C8" s="115" t="s">
+      <c r="C8" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="126" t="s">
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="125" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="3:13">
-      <c r="C9" s="115" t="s">
+      <c r="C9" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="126" t="s">
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="125" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="126"/>
-      <c r="H9" s="126"/>
-      <c r="I9" s="126"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="125"/>
+      <c r="I9" s="125"/>
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="3:13">
-      <c r="C10" s="115" t="s">
+      <c r="C10" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="116"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="140" t="s">
+      <c r="D10" s="115"/>
+      <c r="E10" s="115"/>
+      <c r="F10" s="139" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="140"/>
-      <c r="H10" s="140"/>
-      <c r="I10" s="140"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="139"/>
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="3:13" ht="15.75">
@@ -3360,10 +3367,10 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="3:13">
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="114"/>
+      <c r="D12" s="113"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="3:13">
@@ -3371,17 +3378,17 @@
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="3:13">
-      <c r="C14" s="115" t="s">
+      <c r="C14" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="116"/>
-      <c r="E14" s="144"/>
-      <c r="F14" s="141" t="s">
+      <c r="D14" s="115"/>
+      <c r="E14" s="143"/>
+      <c r="F14" s="140" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="142"/>
-      <c r="H14" s="142"/>
-      <c r="I14" s="143"/>
+      <c r="G14" s="141"/>
+      <c r="H14" s="141"/>
+      <c r="I14" s="142"/>
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="3:13">
@@ -3391,17 +3398,17 @@
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="3:13">
-      <c r="C16" s="115" t="s">
+      <c r="C16" s="114" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="116"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="141" t="s">
+      <c r="D16" s="115"/>
+      <c r="E16" s="143"/>
+      <c r="F16" s="140" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="143"/>
+      <c r="G16" s="141"/>
+      <c r="H16" s="141"/>
+      <c r="I16" s="142"/>
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="3:16">
@@ -3415,54 +3422,54 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="3:16" ht="15" customHeight="1">
-      <c r="C18" s="115" t="s">
+      <c r="C18" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="116"/>
-      <c r="E18" s="116"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="115"/>
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="3:16">
       <c r="C19" s="13"/>
-      <c r="D19" s="127" t="s">
+      <c r="D19" s="126" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="128"/>
-      <c r="F19" s="128"/>
-      <c r="G19" s="128"/>
-      <c r="H19" s="128"/>
-      <c r="I19" s="128"/>
-      <c r="J19" s="129"/>
+      <c r="E19" s="127"/>
+      <c r="F19" s="127"/>
+      <c r="G19" s="127"/>
+      <c r="H19" s="127"/>
+      <c r="I19" s="127"/>
+      <c r="J19" s="128"/>
     </row>
     <row r="20" spans="3:16">
       <c r="C20" s="13"/>
-      <c r="D20" s="130"/>
-      <c r="E20" s="131"/>
-      <c r="F20" s="131"/>
-      <c r="G20" s="131"/>
-      <c r="H20" s="131"/>
-      <c r="I20" s="131"/>
-      <c r="J20" s="132"/>
+      <c r="D20" s="129"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="130"/>
+      <c r="H20" s="130"/>
+      <c r="I20" s="130"/>
+      <c r="J20" s="131"/>
     </row>
     <row r="21" spans="3:16">
       <c r="C21" s="13"/>
-      <c r="D21" s="130"/>
-      <c r="E21" s="131"/>
-      <c r="F21" s="131"/>
-      <c r="G21" s="131"/>
-      <c r="H21" s="131"/>
-      <c r="I21" s="131"/>
-      <c r="J21" s="132"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="130"/>
+      <c r="G21" s="130"/>
+      <c r="H21" s="130"/>
+      <c r="I21" s="130"/>
+      <c r="J21" s="131"/>
     </row>
     <row r="22" spans="3:16">
       <c r="C22" s="13"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="134"/>
-      <c r="G22" s="134"/>
-      <c r="H22" s="134"/>
-      <c r="I22" s="134"/>
-      <c r="J22" s="135"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="133"/>
+      <c r="G22" s="133"/>
+      <c r="H22" s="133"/>
+      <c r="I22" s="133"/>
+      <c r="J22" s="134"/>
     </row>
     <row r="23" spans="3:16" ht="15.75" thickBot="1">
       <c r="C23" s="18"/>
@@ -3475,18 +3482,18 @@
       <c r="J23" s="20"/>
     </row>
     <row r="24" spans="3:16" ht="15.75" thickBot="1">
-      <c r="C24" s="109" t="s">
+      <c r="C24" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="110"/>
-      <c r="E24" s="110"/>
-      <c r="F24" s="110"/>
-      <c r="G24" s="110"/>
-      <c r="H24" s="110"/>
-      <c r="I24" s="111" t="s">
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="109"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="112"/>
+      <c r="J24" s="111"/>
     </row>
     <row r="31" spans="3:16">
       <c r="P31" s="2"/>
@@ -3527,7 +3534,7 @@
       <selection activeCell="F16" sqref="F16:I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="3:13">
       <c r="C3" s="40" t="s">
@@ -3548,24 +3555,24 @@
       <c r="J3" s="45"/>
     </row>
     <row r="4" spans="3:13">
-      <c r="C4" s="159" t="s">
+      <c r="C4" s="158" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="138" t="s">
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="160"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="159"/>
     </row>
     <row r="5" spans="3:13">
-      <c r="C5" s="155" t="s">
+      <c r="C5" s="154" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="114"/>
+      <c r="D5" s="113"/>
       <c r="J5" s="46"/>
     </row>
     <row r="6" spans="3:13">
@@ -3573,45 +3580,45 @@
       <c r="J6" s="46"/>
     </row>
     <row r="7" spans="3:13">
-      <c r="C7" s="145" t="s">
+      <c r="C7" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="126" t="s">
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
       <c r="J7" s="46"/>
     </row>
     <row r="8" spans="3:13">
-      <c r="C8" s="145" t="s">
+      <c r="C8" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="126" t="s">
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
       <c r="J8" s="46"/>
     </row>
     <row r="9" spans="3:13">
-      <c r="C9" s="145" t="s">
+      <c r="C9" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="154" t="s">
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="153" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="140"/>
-      <c r="H9" s="140"/>
-      <c r="I9" s="140"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="139"/>
       <c r="J9" s="46"/>
     </row>
     <row r="10" spans="3:13" ht="15.75">
@@ -3626,10 +3633,10 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="3:13">
-      <c r="C11" s="155" t="s">
+      <c r="C11" s="154" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="113"/>
       <c r="J11" s="46"/>
     </row>
     <row r="12" spans="3:13">
@@ -3637,27 +3644,27 @@
       <c r="J12" s="46"/>
     </row>
     <row r="13" spans="3:13">
-      <c r="C13" s="145" t="s">
+      <c r="C13" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="116"/>
-      <c r="E13" s="156"/>
-      <c r="F13" s="157" t="s">
+      <c r="D13" s="115"/>
+      <c r="E13" s="155"/>
+      <c r="F13" s="156" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="158"/>
-      <c r="H13" s="158"/>
-      <c r="I13" s="158"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="157"/>
+      <c r="I13" s="157"/>
       <c r="J13" s="60"/>
     </row>
     <row r="14" spans="3:13">
       <c r="C14" s="48"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="158"/>
-      <c r="G14" s="158"/>
-      <c r="H14" s="158"/>
-      <c r="I14" s="158"/>
+      <c r="F14" s="157"/>
+      <c r="G14" s="157"/>
+      <c r="H14" s="157"/>
+      <c r="I14" s="157"/>
       <c r="J14" s="60"/>
     </row>
     <row r="15" spans="3:13">
@@ -3667,17 +3674,17 @@
       <c r="J15" s="46"/>
     </row>
     <row r="16" spans="3:13">
-      <c r="C16" s="145" t="s">
+      <c r="C16" s="144" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="116"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="141" t="s">
+      <c r="D16" s="115"/>
+      <c r="E16" s="143"/>
+      <c r="F16" s="140" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="143"/>
+      <c r="G16" s="141"/>
+      <c r="H16" s="141"/>
+      <c r="I16" s="142"/>
       <c r="J16" s="46"/>
     </row>
     <row r="17" spans="3:16">
@@ -3696,12 +3703,12 @@
         <v>60</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="150" t="s">
+      <c r="F18" s="149" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="151"/>
-      <c r="H18" s="151"/>
-      <c r="I18" s="152"/>
+      <c r="G18" s="150"/>
+      <c r="H18" s="150"/>
+      <c r="I18" s="151"/>
       <c r="J18" s="46"/>
     </row>
     <row r="19" spans="3:16">
@@ -3720,12 +3727,12 @@
         <v>62</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="153" t="s">
+      <c r="F20" s="152" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="153"/>
-      <c r="H20" s="153"/>
-      <c r="I20" s="153"/>
+      <c r="G20" s="152"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="152"/>
       <c r="J20" s="55"/>
       <c r="L20" s="37"/>
     </row>
@@ -3733,10 +3740,10 @@
       <c r="C21" s="48"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="153"/>
-      <c r="G21" s="153"/>
-      <c r="H21" s="153"/>
-      <c r="I21" s="153"/>
+      <c r="F21" s="152"/>
+      <c r="G21" s="152"/>
+      <c r="H21" s="152"/>
+      <c r="I21" s="152"/>
       <c r="J21" s="61"/>
       <c r="L21" s="39"/>
     </row>
@@ -3752,18 +3759,18 @@
       <c r="L22" s="39"/>
     </row>
     <row r="23" spans="3:16">
-      <c r="C23" s="146" t="s">
+      <c r="C23" s="145" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="147"/>
-      <c r="E23" s="147"/>
-      <c r="F23" s="147"/>
-      <c r="G23" s="147"/>
-      <c r="H23" s="147"/>
-      <c r="I23" s="148" t="s">
+      <c r="D23" s="146"/>
+      <c r="E23" s="146"/>
+      <c r="F23" s="146"/>
+      <c r="G23" s="146"/>
+      <c r="H23" s="146"/>
+      <c r="I23" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="149"/>
+      <c r="J23" s="148"/>
       <c r="L23" s="39"/>
     </row>
     <row r="24" spans="3:16">
@@ -3806,7 +3813,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="3:10">
       <c r="C3" s="40" t="s">
@@ -3827,24 +3834,24 @@
       <c r="J3" s="45"/>
     </row>
     <row r="4" spans="3:10">
-      <c r="C4" s="159" t="s">
+      <c r="C4" s="158" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="138" t="s">
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="160"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="159"/>
     </row>
     <row r="5" spans="3:10">
-      <c r="C5" s="170" t="s">
+      <c r="C5" s="169" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="171"/>
+      <c r="D5" s="170"/>
       <c r="J5" s="46"/>
     </row>
     <row r="6" spans="3:10">
@@ -3852,45 +3859,45 @@
       <c r="J6" s="46"/>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="145" t="s">
+      <c r="C7" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="126" t="s">
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
       <c r="J7" s="46"/>
     </row>
     <row r="8" spans="3:10">
-      <c r="C8" s="145" t="s">
+      <c r="C8" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="126" t="s">
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
       <c r="J8" s="46"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="145" t="s">
+      <c r="C9" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="154" t="s">
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="153" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="154"/>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
+      <c r="G9" s="153"/>
+      <c r="H9" s="153"/>
+      <c r="I9" s="153"/>
       <c r="J9" s="46"/>
     </row>
     <row r="10" spans="3:10">
@@ -3904,10 +3911,10 @@
       <c r="J10" s="46"/>
     </row>
     <row r="11" spans="3:10">
-      <c r="C11" s="155" t="s">
+      <c r="C11" s="154" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="113"/>
       <c r="E11" s="10"/>
       <c r="F11" s="35"/>
       <c r="G11" s="34"/>
@@ -3931,12 +3938,12 @@
         <v>38</v>
       </c>
       <c r="E13" s="35"/>
-      <c r="F13" s="176" t="s">
+      <c r="F13" s="175" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="177"/>
-      <c r="H13" s="177"/>
-      <c r="I13" s="178"/>
+      <c r="G13" s="176"/>
+      <c r="H13" s="176"/>
+      <c r="I13" s="177"/>
       <c r="J13" s="49"/>
     </row>
     <row r="14" spans="3:10">
@@ -3945,12 +3952,12 @@
         <v>40</v>
       </c>
       <c r="E14" s="36"/>
-      <c r="F14" s="176" t="s">
+      <c r="F14" s="175" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="177"/>
-      <c r="H14" s="177"/>
-      <c r="I14" s="178"/>
+      <c r="G14" s="176"/>
+      <c r="H14" s="176"/>
+      <c r="I14" s="177"/>
       <c r="J14" s="50"/>
     </row>
     <row r="15" spans="3:10">
@@ -3959,12 +3966,12 @@
         <v>42</v>
       </c>
       <c r="E15" s="36"/>
-      <c r="F15" s="176" t="s">
+      <c r="F15" s="175" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="177"/>
-      <c r="H15" s="177"/>
-      <c r="I15" s="178"/>
+      <c r="G15" s="176"/>
+      <c r="H15" s="176"/>
+      <c r="I15" s="177"/>
       <c r="J15" s="50"/>
     </row>
     <row r="16" spans="3:10">
@@ -3973,12 +3980,12 @@
         <v>68</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="179" t="s">
+      <c r="F16" s="178" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="180"/>
-      <c r="H16" s="180"/>
-      <c r="I16" s="181"/>
+      <c r="G16" s="179"/>
+      <c r="H16" s="179"/>
+      <c r="I16" s="180"/>
       <c r="J16" s="51"/>
     </row>
     <row r="17" spans="3:13" ht="15.75">
@@ -3993,10 +4000,10 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="3:13">
-      <c r="C18" s="170" t="s">
+      <c r="C18" s="169" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="171"/>
+      <c r="D18" s="170"/>
       <c r="J18" s="46"/>
     </row>
     <row r="19" spans="3:13">
@@ -4004,17 +4011,17 @@
       <c r="J19" s="46"/>
     </row>
     <row r="20" spans="3:13">
-      <c r="C20" s="145" t="s">
+      <c r="C20" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="116"/>
-      <c r="E20" s="144"/>
-      <c r="F20" s="167" t="s">
+      <c r="D20" s="115"/>
+      <c r="E20" s="143"/>
+      <c r="F20" s="166" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="151"/>
-      <c r="H20" s="151"/>
-      <c r="I20" s="168"/>
+      <c r="G20" s="150"/>
+      <c r="H20" s="150"/>
+      <c r="I20" s="167"/>
       <c r="J20" s="60"/>
     </row>
     <row r="21" spans="3:13">
@@ -4024,17 +4031,17 @@
       <c r="J21" s="46"/>
     </row>
     <row r="22" spans="3:13">
-      <c r="C22" s="145" t="s">
+      <c r="C22" s="144" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="116"/>
-      <c r="E22" s="144"/>
-      <c r="F22" s="141" t="s">
+      <c r="D22" s="115"/>
+      <c r="E22" s="143"/>
+      <c r="F22" s="140" t="s">
         <v>74</v>
       </c>
-      <c r="G22" s="142"/>
-      <c r="H22" s="142"/>
-      <c r="I22" s="143"/>
+      <c r="G22" s="141"/>
+      <c r="H22" s="141"/>
+      <c r="I22" s="142"/>
       <c r="J22" s="46"/>
     </row>
     <row r="23" spans="3:13">
@@ -4053,22 +4060,22 @@
         <v>75</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="F24" s="161" t="s">
+      <c r="F24" s="160" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="162"/>
-      <c r="H24" s="162"/>
-      <c r="I24" s="163"/>
+      <c r="G24" s="161"/>
+      <c r="H24" s="161"/>
+      <c r="I24" s="162"/>
       <c r="J24" s="46"/>
     </row>
     <row r="25" spans="3:13">
       <c r="C25" s="48"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="164"/>
-      <c r="G25" s="165"/>
-      <c r="H25" s="165"/>
-      <c r="I25" s="166"/>
+      <c r="F25" s="163"/>
+      <c r="G25" s="164"/>
+      <c r="H25" s="164"/>
+      <c r="I25" s="165"/>
       <c r="J25" s="46"/>
     </row>
     <row r="26" spans="3:13">
@@ -4082,17 +4089,17 @@
       <c r="J26" s="54"/>
     </row>
     <row r="27" spans="3:13">
-      <c r="C27" s="145" t="s">
+      <c r="C27" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="116"/>
-      <c r="E27" s="156"/>
-      <c r="F27" s="169" t="s">
+      <c r="D27" s="115"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="168" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="153"/>
-      <c r="H27" s="153"/>
-      <c r="I27" s="153"/>
+      <c r="G27" s="152"/>
+      <c r="H27" s="152"/>
+      <c r="I27" s="152"/>
       <c r="J27" s="55"/>
       <c r="L27" s="38"/>
     </row>
@@ -4100,10 +4107,10 @@
       <c r="C28" s="48"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="153"/>
-      <c r="G28" s="153"/>
-      <c r="H28" s="153"/>
-      <c r="I28" s="153"/>
+      <c r="F28" s="152"/>
+      <c r="G28" s="152"/>
+      <c r="H28" s="152"/>
+      <c r="I28" s="152"/>
       <c r="J28" s="46"/>
       <c r="L28" s="39"/>
     </row>
@@ -4119,17 +4126,17 @@
       <c r="L29" s="39"/>
     </row>
     <row r="30" spans="3:13" ht="13.5" customHeight="1">
-      <c r="C30" s="173" t="s">
+      <c r="C30" s="172" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="174"/>
-      <c r="E30" s="175"/>
-      <c r="F30" s="169" t="s">
+      <c r="D30" s="173"/>
+      <c r="E30" s="174"/>
+      <c r="F30" s="168" t="s">
         <v>80</v>
       </c>
-      <c r="G30" s="153"/>
-      <c r="H30" s="153"/>
-      <c r="I30" s="153"/>
+      <c r="G30" s="152"/>
+      <c r="H30" s="152"/>
+      <c r="I30" s="152"/>
       <c r="J30" s="46"/>
       <c r="L30" s="39"/>
     </row>
@@ -4137,10 +4144,10 @@
       <c r="C31" s="63"/>
       <c r="D31" s="62"/>
       <c r="E31" s="64"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="153"/>
-      <c r="H31" s="153"/>
-      <c r="I31" s="153"/>
+      <c r="F31" s="152"/>
+      <c r="G31" s="152"/>
+      <c r="H31" s="152"/>
+      <c r="I31" s="152"/>
       <c r="J31" s="46"/>
       <c r="L31" s="39"/>
     </row>
@@ -4156,18 +4163,18 @@
       <c r="L32" s="38"/>
     </row>
     <row r="33" spans="3:16">
-      <c r="C33" s="146" t="s">
+      <c r="C33" s="145" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="147"/>
-      <c r="E33" s="147"/>
-      <c r="F33" s="147"/>
-      <c r="G33" s="147"/>
-      <c r="H33" s="147"/>
-      <c r="I33" s="148" t="s">
+      <c r="D33" s="146"/>
+      <c r="E33" s="146"/>
+      <c r="F33" s="146"/>
+      <c r="G33" s="146"/>
+      <c r="H33" s="146"/>
+      <c r="I33" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="J33" s="172"/>
+      <c r="J33" s="171"/>
     </row>
     <row r="40" spans="3:16" ht="15" customHeight="1">
       <c r="P40" s="2"/>
@@ -4210,11 +4217,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4241AF6E-F419-42F8-AF45-EBCD4A961F68}">
   <dimension ref="D4:K50"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -4238,18 +4245,18 @@
       <c r="K4" s="45"/>
     </row>
     <row r="5" spans="4:11">
-      <c r="D5" s="159" t="s">
+      <c r="D5" s="158" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="137"/>
-      <c r="F5" s="137"/>
-      <c r="G5" s="137"/>
-      <c r="H5" s="138" t="s">
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="137" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="138"/>
-      <c r="J5" s="138"/>
-      <c r="K5" s="160"/>
+      <c r="I5" s="137"/>
+      <c r="J5" s="137"/>
+      <c r="K5" s="159"/>
     </row>
     <row r="6" spans="4:11" hidden="1">
       <c r="D6" s="48"/>
@@ -4262,498 +4269,498 @@
       <c r="K6" s="60"/>
     </row>
     <row r="7" spans="4:11">
-      <c r="D7" s="184"/>
-      <c r="E7" s="185"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
-      <c r="K7" s="103"/>
+      <c r="D7" s="182"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="99"/>
     </row>
     <row r="8" spans="4:11">
-      <c r="D8" s="182" t="s">
+      <c r="D8" s="181" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="183"/>
-      <c r="F8" s="183"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="76"/>
+      <c r="E8" s="243"/>
+      <c r="F8" s="243"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="74"/>
     </row>
     <row r="9" spans="4:11">
-      <c r="D9" s="77"/>
+      <c r="D9" s="75"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="35"/>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
-      <c r="K9" s="76"/>
+      <c r="K9" s="74"/>
     </row>
     <row r="10" spans="4:11">
-      <c r="D10" s="217" t="s">
+      <c r="D10" s="215" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="218"/>
-      <c r="F10" s="218"/>
-      <c r="G10" s="186" t="s">
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="184" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="187"/>
-      <c r="I10" s="187"/>
-      <c r="J10" s="188"/>
-      <c r="K10" s="78"/>
+      <c r="H10" s="185"/>
+      <c r="I10" s="185"/>
+      <c r="J10" s="186"/>
+      <c r="K10" s="76"/>
     </row>
     <row r="11" spans="4:11">
-      <c r="D11" s="193" t="s">
+      <c r="D11" s="191" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
-      <c r="G11" s="176" t="s">
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
+      <c r="G11" s="175" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="177"/>
-      <c r="I11" s="177"/>
-      <c r="J11" s="178"/>
-      <c r="K11" s="79"/>
+      <c r="H11" s="176"/>
+      <c r="I11" s="176"/>
+      <c r="J11" s="177"/>
+      <c r="K11" s="77"/>
     </row>
     <row r="12" spans="4:11">
-      <c r="D12" s="217" t="s">
+      <c r="D12" s="215" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="183"/>
-      <c r="F12" s="183"/>
-      <c r="G12" s="222" t="s">
+      <c r="E12" s="243"/>
+      <c r="F12" s="243"/>
+      <c r="G12" s="220" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="223"/>
-      <c r="I12" s="223"/>
-      <c r="J12" s="224"/>
-      <c r="K12" s="79"/>
+      <c r="H12" s="221"/>
+      <c r="I12" s="221"/>
+      <c r="J12" s="222"/>
+      <c r="K12" s="77"/>
     </row>
     <row r="13" spans="4:11">
-      <c r="D13" s="80"/>
+      <c r="D13" s="78"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="65"/>
       <c r="H13" s="65"/>
       <c r="I13" s="65"/>
       <c r="J13" s="65"/>
-      <c r="K13" s="81"/>
+      <c r="K13" s="79"/>
     </row>
     <row r="14" spans="4:11">
-      <c r="D14" s="182" t="s">
+      <c r="D14" s="181" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="194"/>
-      <c r="F14" s="194"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="126"/>
-      <c r="J14" s="126"/>
-      <c r="K14" s="76"/>
+      <c r="E14" s="192"/>
+      <c r="F14" s="192"/>
+      <c r="G14" s="125"/>
+      <c r="H14" s="125"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="125"/>
+      <c r="K14" s="74"/>
     </row>
     <row r="15" spans="4:11">
-      <c r="D15" s="82"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="76"/>
+      <c r="D15" s="80"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="74"/>
     </row>
     <row r="16" spans="4:11">
-      <c r="D16" s="193" t="s">
+      <c r="D16" s="191" t="s">
         <v>91</v>
       </c>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="76"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="115"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="74"/>
     </row>
     <row r="17" spans="4:11">
-      <c r="D17" s="77"/>
+      <c r="D17" s="75"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="76"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="74"/>
     </row>
     <row r="18" spans="4:11" ht="15" customHeight="1">
-      <c r="D18" s="219" t="s">
+      <c r="D18" s="217" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="220"/>
-      <c r="F18" s="221"/>
-      <c r="G18" s="195" t="s">
+      <c r="E18" s="218"/>
+      <c r="F18" s="219"/>
+      <c r="G18" s="193" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="196"/>
-      <c r="I18" s="196"/>
-      <c r="J18" s="197"/>
-      <c r="K18" s="76"/>
+      <c r="H18" s="194"/>
+      <c r="I18" s="194"/>
+      <c r="J18" s="195"/>
+      <c r="K18" s="74"/>
     </row>
     <row r="19" spans="4:11">
-      <c r="D19" s="86"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="198"/>
-      <c r="H19" s="199"/>
-      <c r="I19" s="199"/>
-      <c r="J19" s="200"/>
-      <c r="K19" s="76"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="196"/>
+      <c r="H19" s="197"/>
+      <c r="I19" s="197"/>
+      <c r="J19" s="198"/>
+      <c r="K19" s="74"/>
     </row>
     <row r="20" spans="4:11">
-      <c r="D20" s="86"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
-      <c r="K20" s="76"/>
+      <c r="K20" s="74"/>
     </row>
     <row r="21" spans="4:11" ht="15" customHeight="1">
-      <c r="D21" s="219" t="s">
+      <c r="D21" s="217" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="220"/>
-      <c r="F21" s="221"/>
-      <c r="G21" s="201" t="s">
+      <c r="E21" s="218"/>
+      <c r="F21" s="219"/>
+      <c r="G21" s="199" t="s">
         <v>95</v>
       </c>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202"/>
-      <c r="J21" s="203"/>
-      <c r="K21" s="76"/>
+      <c r="H21" s="200"/>
+      <c r="I21" s="200"/>
+      <c r="J21" s="201"/>
+      <c r="K21" s="74"/>
     </row>
     <row r="22" spans="4:11">
-      <c r="D22" s="86"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="204"/>
-      <c r="H22" s="205"/>
-      <c r="I22" s="205"/>
-      <c r="J22" s="206"/>
-      <c r="K22" s="76"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="202"/>
+      <c r="H22" s="203"/>
+      <c r="I22" s="203"/>
+      <c r="J22" s="204"/>
+      <c r="K22" s="74"/>
     </row>
     <row r="23" spans="4:11">
-      <c r="D23" s="86"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
-      <c r="K23" s="76"/>
+      <c r="K23" s="74"/>
     </row>
     <row r="24" spans="4:11">
-      <c r="D24" s="215" t="s">
+      <c r="D24" s="213" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="216"/>
-      <c r="F24" s="216"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="96"/>
+      <c r="E24" s="214"/>
+      <c r="F24" s="214"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="93"/>
     </row>
     <row r="25" spans="4:11">
-      <c r="D25" s="86"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-      <c r="K25" s="76"/>
+      <c r="K25" s="74"/>
     </row>
     <row r="26" spans="4:11" ht="15" customHeight="1">
-      <c r="D26" s="219" t="s">
+      <c r="D26" s="217" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="220"/>
-      <c r="F26" s="221"/>
-      <c r="G26" s="209" t="s">
+      <c r="E26" s="218"/>
+      <c r="F26" s="219"/>
+      <c r="G26" s="207" t="s">
         <v>97</v>
       </c>
-      <c r="H26" s="210"/>
-      <c r="I26" s="210"/>
-      <c r="J26" s="211"/>
-      <c r="K26" s="76"/>
+      <c r="H26" s="208"/>
+      <c r="I26" s="208"/>
+      <c r="J26" s="209"/>
+      <c r="K26" s="74"/>
     </row>
     <row r="27" spans="4:11">
-      <c r="D27" s="86"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="212"/>
-      <c r="H27" s="213"/>
-      <c r="I27" s="213"/>
-      <c r="J27" s="214"/>
-      <c r="K27" s="76"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="85"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="210"/>
+      <c r="H27" s="211"/>
+      <c r="I27" s="211"/>
+      <c r="J27" s="212"/>
+      <c r="K27" s="74"/>
     </row>
     <row r="28" spans="4:11">
-      <c r="D28" s="86"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="88"/>
-      <c r="H28" s="88"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="76"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="85"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="74"/>
     </row>
     <row r="29" spans="4:11">
-      <c r="D29" s="86"/>
-      <c r="E29" s="220" t="s">
+      <c r="D29" s="84"/>
+      <c r="E29" s="218" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="220"/>
-      <c r="G29" s="201" t="s">
+      <c r="F29" s="218"/>
+      <c r="G29" s="199" t="s">
         <v>98</v>
       </c>
-      <c r="H29" s="202"/>
-      <c r="I29" s="202"/>
-      <c r="J29" s="203"/>
-      <c r="K29" s="76"/>
+      <c r="H29" s="200"/>
+      <c r="I29" s="200"/>
+      <c r="J29" s="201"/>
+      <c r="K29" s="74"/>
     </row>
     <row r="30" spans="4:11">
-      <c r="D30" s="86"/>
-      <c r="E30" s="85"/>
-      <c r="F30" s="85"/>
-      <c r="G30" s="204"/>
-      <c r="H30" s="205"/>
-      <c r="I30" s="205"/>
-      <c r="J30" s="206"/>
-      <c r="K30" s="76"/>
+      <c r="D30" s="84"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="202"/>
+      <c r="H30" s="203"/>
+      <c r="I30" s="203"/>
+      <c r="J30" s="204"/>
+      <c r="K30" s="74"/>
     </row>
     <row r="31" spans="4:11">
-      <c r="D31" s="86"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="85"/>
+      <c r="F31" s="85"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
-      <c r="K31" s="76"/>
+      <c r="K31" s="74"/>
     </row>
     <row r="32" spans="4:11">
-      <c r="D32" s="207" t="s">
+      <c r="D32" s="205" t="s">
         <v>99</v>
       </c>
-      <c r="E32" s="208"/>
-      <c r="F32" s="208"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="96"/>
+      <c r="E32" s="206"/>
+      <c r="F32" s="206"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="93"/>
     </row>
     <row r="33" spans="4:11">
-      <c r="D33" s="86"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="85"/>
+      <c r="F33" s="85"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
-      <c r="K33" s="76"/>
+      <c r="K33" s="74"/>
     </row>
     <row r="34" spans="4:11" ht="15" customHeight="1">
-      <c r="D34" s="219" t="s">
+      <c r="D34" s="217" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="220"/>
-      <c r="F34" s="221"/>
-      <c r="G34" s="209" t="s">
+      <c r="E34" s="218"/>
+      <c r="F34" s="219"/>
+      <c r="G34" s="207" t="s">
         <v>100</v>
       </c>
-      <c r="H34" s="210"/>
-      <c r="I34" s="210"/>
-      <c r="J34" s="211"/>
-      <c r="K34" s="76"/>
+      <c r="H34" s="208"/>
+      <c r="I34" s="208"/>
+      <c r="J34" s="209"/>
+      <c r="K34" s="74"/>
     </row>
     <row r="35" spans="4:11">
-      <c r="D35" s="86"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="212"/>
-      <c r="H35" s="213"/>
-      <c r="I35" s="213"/>
-      <c r="J35" s="214"/>
-      <c r="K35" s="76"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="210"/>
+      <c r="H35" s="211"/>
+      <c r="I35" s="211"/>
+      <c r="J35" s="212"/>
+      <c r="K35" s="74"/>
     </row>
     <row r="36" spans="4:11">
-      <c r="D36" s="86"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="88"/>
-      <c r="H36" s="88"/>
-      <c r="I36" s="88"/>
-      <c r="J36" s="88"/>
-      <c r="K36" s="76"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="86"/>
+      <c r="I36" s="86"/>
+      <c r="J36" s="86"/>
+      <c r="K36" s="74"/>
     </row>
     <row r="37" spans="4:11" ht="15" customHeight="1">
-      <c r="D37" s="219" t="s">
+      <c r="D37" s="217" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="220"/>
-      <c r="F37" s="221"/>
-      <c r="G37" s="201" t="s">
+      <c r="E37" s="218"/>
+      <c r="F37" s="219"/>
+      <c r="G37" s="199" t="s">
         <v>101</v>
       </c>
-      <c r="H37" s="202"/>
-      <c r="I37" s="202"/>
-      <c r="J37" s="203"/>
-      <c r="K37" s="76"/>
+      <c r="H37" s="200"/>
+      <c r="I37" s="200"/>
+      <c r="J37" s="201"/>
+      <c r="K37" s="74"/>
     </row>
     <row r="38" spans="4:11">
-      <c r="D38" s="86"/>
-      <c r="E38" s="85"/>
-      <c r="F38" s="85"/>
-      <c r="G38" s="204"/>
-      <c r="H38" s="205"/>
-      <c r="I38" s="205"/>
-      <c r="J38" s="206"/>
-      <c r="K38" s="76"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="202"/>
+      <c r="H38" s="203"/>
+      <c r="I38" s="203"/>
+      <c r="J38" s="204"/>
+      <c r="K38" s="74"/>
     </row>
     <row r="39" spans="4:11">
-      <c r="D39" s="86"/>
-      <c r="E39" s="87"/>
-      <c r="F39" s="87"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="85"/>
+      <c r="F39" s="85"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
-      <c r="K39" s="76"/>
+      <c r="K39" s="74"/>
     </row>
     <row r="40" spans="4:11">
-      <c r="D40" s="82"/>
-      <c r="G40" s="83"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="83"/>
-      <c r="J40" s="83"/>
-      <c r="K40" s="76"/>
+      <c r="D40" s="80"/>
+      <c r="G40" s="81"/>
+      <c r="H40" s="81"/>
+      <c r="I40" s="81"/>
+      <c r="J40" s="81"/>
+      <c r="K40" s="74"/>
     </row>
     <row r="41" spans="4:11">
-      <c r="D41" s="97" t="s">
+      <c r="D41" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="E41" s="71"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="67"/>
-      <c r="H41" s="67"/>
-      <c r="I41" s="67"/>
-      <c r="J41" s="67"/>
-      <c r="K41" s="96"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="66"/>
+      <c r="J41" s="66"/>
+      <c r="K41" s="93"/>
     </row>
     <row r="42" spans="4:11">
-      <c r="D42" s="82"/>
-      <c r="G42" s="83"/>
-      <c r="H42" s="83"/>
-      <c r="I42" s="83"/>
-      <c r="J42" s="83"/>
-      <c r="K42" s="76"/>
+      <c r="D42" s="80"/>
+      <c r="G42" s="81"/>
+      <c r="H42" s="81"/>
+      <c r="I42" s="81"/>
+      <c r="J42" s="81"/>
+      <c r="K42" s="74"/>
     </row>
     <row r="43" spans="4:11">
-      <c r="D43" s="82"/>
-      <c r="E43" s="218" t="s">
+      <c r="D43" s="80"/>
+      <c r="E43" s="216" t="s">
         <v>103</v>
       </c>
-      <c r="F43" s="218"/>
-      <c r="G43" s="150" t="s">
+      <c r="F43" s="216"/>
+      <c r="G43" s="149" t="s">
         <v>104</v>
       </c>
-      <c r="H43" s="151"/>
-      <c r="I43" s="151"/>
-      <c r="J43" s="152"/>
-      <c r="K43" s="76"/>
+      <c r="H43" s="150"/>
+      <c r="I43" s="150"/>
+      <c r="J43" s="151"/>
+      <c r="K43" s="74"/>
     </row>
     <row r="44" spans="4:11">
-      <c r="D44" s="82"/>
-      <c r="G44" s="83"/>
-      <c r="H44" s="83"/>
-      <c r="I44" s="83"/>
-      <c r="J44" s="83"/>
-      <c r="K44" s="76"/>
+      <c r="D44" s="80"/>
+      <c r="G44" s="81"/>
+      <c r="H44" s="81"/>
+      <c r="I44" s="81"/>
+      <c r="J44" s="81"/>
+      <c r="K44" s="74"/>
     </row>
     <row r="45" spans="4:11">
-      <c r="D45" s="82"/>
-      <c r="E45" s="218" t="s">
+      <c r="D45" s="80"/>
+      <c r="E45" s="216" t="s">
         <v>105</v>
       </c>
-      <c r="F45" s="218"/>
-      <c r="G45" s="150" t="s">
+      <c r="F45" s="216"/>
+      <c r="G45" s="149" t="s">
         <v>106</v>
       </c>
-      <c r="H45" s="151"/>
-      <c r="I45" s="151"/>
-      <c r="J45" s="152"/>
-      <c r="K45" s="76"/>
+      <c r="H45" s="150"/>
+      <c r="I45" s="150"/>
+      <c r="J45" s="151"/>
+      <c r="K45" s="74"/>
     </row>
     <row r="46" spans="4:11">
-      <c r="D46" s="82"/>
-      <c r="F46" s="104"/>
-      <c r="G46" s="83"/>
-      <c r="H46" s="83"/>
-      <c r="I46" s="83"/>
-      <c r="J46" s="83"/>
-      <c r="K46" s="76"/>
+      <c r="D46" s="80"/>
+      <c r="F46" s="100"/>
+      <c r="G46" s="81"/>
+      <c r="H46" s="81"/>
+      <c r="I46" s="81"/>
+      <c r="J46" s="81"/>
+      <c r="K46" s="74"/>
     </row>
     <row r="47" spans="4:11">
-      <c r="D47" s="217" t="s">
+      <c r="D47" s="215" t="s">
         <v>107</v>
       </c>
-      <c r="E47" s="218"/>
-      <c r="F47" s="218"/>
-      <c r="G47" s="150" t="s">
+      <c r="E47" s="216"/>
+      <c r="F47" s="216"/>
+      <c r="G47" s="149" t="s">
         <v>108</v>
       </c>
-      <c r="H47" s="151"/>
-      <c r="I47" s="151"/>
-      <c r="J47" s="152"/>
-      <c r="K47" s="76"/>
+      <c r="H47" s="150"/>
+      <c r="I47" s="150"/>
+      <c r="J47" s="151"/>
+      <c r="K47" s="74"/>
     </row>
     <row r="48" spans="4:11">
-      <c r="D48" s="82"/>
-      <c r="F48" s="104"/>
-      <c r="G48" s="83"/>
-      <c r="H48" s="83"/>
-      <c r="I48" s="83"/>
-      <c r="J48" s="83"/>
-      <c r="K48" s="76"/>
+      <c r="D48" s="80"/>
+      <c r="F48" s="100"/>
+      <c r="G48" s="81"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="81"/>
+      <c r="J48" s="81"/>
+      <c r="K48" s="74"/>
     </row>
     <row r="49" spans="4:11">
-      <c r="D49" s="105"/>
-      <c r="E49" s="106"/>
-      <c r="F49" s="106"/>
-      <c r="G49" s="106"/>
-      <c r="H49" s="106"/>
-      <c r="I49" s="106"/>
-      <c r="J49" s="106"/>
-      <c r="K49" s="107"/>
+      <c r="D49" s="101"/>
+      <c r="E49" s="102"/>
+      <c r="F49" s="102"/>
+      <c r="G49" s="102"/>
+      <c r="H49" s="102"/>
+      <c r="I49" s="102"/>
+      <c r="J49" s="102"/>
+      <c r="K49" s="103"/>
     </row>
     <row r="50" spans="4:11">
-      <c r="D50" s="189" t="s">
+      <c r="D50" s="187" t="s">
         <v>109</v>
       </c>
-      <c r="E50" s="190"/>
-      <c r="F50" s="190"/>
-      <c r="G50" s="190"/>
-      <c r="H50" s="190"/>
-      <c r="I50" s="190"/>
-      <c r="J50" s="191" t="s">
+      <c r="E50" s="188"/>
+      <c r="F50" s="188"/>
+      <c r="G50" s="188"/>
+      <c r="H50" s="188"/>
+      <c r="I50" s="188"/>
+      <c r="J50" s="189" t="s">
         <v>19</v>
       </c>
-      <c r="K50" s="192"/>
+      <c r="K50" s="190"/>
     </row>
   </sheetData>
   <mergeCells count="36">
@@ -4800,384 +4807,297 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067811A3-40C7-46FF-88F1-AD79AA6922DE}">
-  <dimension ref="C5:J34"/>
+  <dimension ref="D5:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10">
-      <c r="C5" s="40" t="s">
+    <row r="5" spans="4:11">
+      <c r="D5" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="E5" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="42"/>
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="42"/>
+      <c r="I5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="44">
+      <c r="J5" s="44">
         <v>45323</v>
       </c>
-      <c r="J5" s="45"/>
-    </row>
-    <row r="6" spans="3:10">
-      <c r="C6" s="232" t="s">
+      <c r="K5" s="45"/>
+    </row>
+    <row r="6" spans="4:11">
+      <c r="D6" s="230" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="233"/>
-      <c r="E6" s="233"/>
-      <c r="F6" s="233"/>
-      <c r="G6" s="234" t="s">
+      <c r="E6" s="231"/>
+      <c r="F6" s="231"/>
+      <c r="G6" s="231"/>
+      <c r="H6" s="232" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="234"/>
-      <c r="I6" s="234"/>
-      <c r="J6" s="235"/>
-    </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="184"/>
-      <c r="D7" s="185"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="75"/>
-    </row>
-    <row r="8" spans="3:10">
-      <c r="C8" s="182" t="s">
+      <c r="I6" s="232"/>
+      <c r="J6" s="232"/>
+      <c r="K6" s="233"/>
+    </row>
+    <row r="7" spans="4:11">
+      <c r="D7" s="182"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="73"/>
+    </row>
+    <row r="8" spans="4:11">
+      <c r="D8" s="181" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="183"/>
-      <c r="E8" s="183"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="76"/>
-    </row>
-    <row r="9" spans="3:10">
-      <c r="C9" s="77"/>
-      <c r="D9" s="10"/>
+      <c r="E8" s="243"/>
+      <c r="F8" s="243"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="74"/>
+    </row>
+    <row r="9" spans="4:11">
+      <c r="D9" s="75"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="34"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="35"/>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
-      <c r="J9" s="76"/>
-    </row>
-    <row r="10" spans="3:10">
-      <c r="C10" s="217" t="s">
+      <c r="J9" s="34"/>
+      <c r="K9" s="74"/>
+    </row>
+    <row r="10" spans="4:11">
+      <c r="D10" s="215" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="218"/>
-      <c r="E10" s="218"/>
-      <c r="F10" s="186" t="s">
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="184" t="s">
         <v>112</v>
       </c>
-      <c r="G10" s="187"/>
-      <c r="H10" s="187"/>
-      <c r="I10" s="188"/>
-      <c r="J10" s="78"/>
-    </row>
-    <row r="11" spans="3:10">
-      <c r="C11" s="193" t="s">
+      <c r="H10" s="185"/>
+      <c r="I10" s="185"/>
+      <c r="J10" s="186"/>
+      <c r="K10" s="76"/>
+    </row>
+    <row r="11" spans="4:11">
+      <c r="D11" s="191" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="176" t="s">
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
+      <c r="G11" s="175" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="177"/>
-      <c r="H11" s="177"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="79"/>
-    </row>
-    <row r="12" spans="3:10">
-      <c r="C12" s="217" t="s">
+      <c r="H11" s="176"/>
+      <c r="I11" s="176"/>
+      <c r="J11" s="177"/>
+      <c r="K11" s="77"/>
+    </row>
+    <row r="12" spans="4:11">
+      <c r="D12" s="215" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="183"/>
-      <c r="E12" s="183"/>
-      <c r="F12" s="222" t="s">
+      <c r="E12" s="243"/>
+      <c r="F12" s="243"/>
+      <c r="G12" s="220" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="223"/>
-      <c r="H12" s="223"/>
-      <c r="I12" s="224"/>
-      <c r="J12" s="79"/>
-    </row>
-    <row r="13" spans="3:10">
-      <c r="C13" s="80"/>
-      <c r="D13" s="9"/>
+      <c r="H12" s="221"/>
+      <c r="I12" s="221"/>
+      <c r="J12" s="222"/>
+      <c r="K12" s="77"/>
+    </row>
+    <row r="13" spans="4:11">
+      <c r="D13" s="78"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="65"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="65"/>
       <c r="H13" s="65"/>
       <c r="I13" s="65"/>
-      <c r="J13" s="81"/>
-    </row>
-    <row r="14" spans="3:10">
-      <c r="C14" s="225" t="s">
+      <c r="J13" s="65"/>
+      <c r="K13" s="79"/>
+    </row>
+    <row r="14" spans="4:11">
+      <c r="D14" s="223" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="116"/>
-      <c r="E14" s="116"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="126"/>
-      <c r="J14" s="76"/>
-    </row>
-    <row r="15" spans="3:10">
-      <c r="C15" s="82"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="76"/>
-    </row>
-    <row r="16" spans="3:10">
-      <c r="C16" s="219" t="s">
+      <c r="E14" s="115"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="125"/>
+      <c r="H14" s="125"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="125"/>
+      <c r="K14" s="74"/>
+    </row>
+    <row r="15" spans="4:11">
+      <c r="D15" s="80"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="74"/>
+    </row>
+    <row r="16" spans="4:11" ht="15" customHeight="1">
+      <c r="D16" s="217" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="220"/>
-      <c r="E16" s="221"/>
-      <c r="F16" s="195" t="s">
+      <c r="E16" s="218"/>
+      <c r="F16" s="219"/>
+      <c r="G16" s="193" t="s">
         <v>115</v>
       </c>
-      <c r="G16" s="226"/>
-      <c r="H16" s="226"/>
-      <c r="I16" s="227"/>
-      <c r="J16" s="76"/>
-    </row>
-    <row r="17" spans="3:10">
-      <c r="C17" s="84"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="228"/>
-      <c r="G17" s="229"/>
-      <c r="H17" s="229"/>
-      <c r="I17" s="230"/>
-      <c r="J17" s="76"/>
-    </row>
-    <row r="18" spans="3:10">
-      <c r="C18" s="86"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="88"/>
-      <c r="G18" s="88"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="76"/>
-    </row>
-    <row r="19" spans="3:10">
-      <c r="C19" s="86"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="88"/>
-      <c r="J19" s="76"/>
-    </row>
-    <row r="20" spans="3:10" s="95" customFormat="1">
-      <c r="C20" s="97" t="s">
+      <c r="H16" s="224"/>
+      <c r="I16" s="224"/>
+      <c r="J16" s="225"/>
+      <c r="K16" s="74"/>
+    </row>
+    <row r="17" spans="4:11">
+      <c r="D17" s="82"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="226"/>
+      <c r="H17" s="227"/>
+      <c r="I17" s="227"/>
+      <c r="J17" s="228"/>
+      <c r="K17" s="74"/>
+    </row>
+    <row r="18" spans="4:11">
+      <c r="D18" s="84"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="74"/>
+    </row>
+    <row r="19" spans="4:11">
+      <c r="D19" s="84"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="86"/>
+      <c r="K19" s="74"/>
+    </row>
+    <row r="20" spans="4:11" s="92" customFormat="1">
+      <c r="D20" s="229" t="s">
         <v>116</v>
       </c>
-      <c r="D20" s="98"/>
-      <c r="E20" s="98"/>
-      <c r="F20" s="66"/>
+      <c r="E20" s="206"/>
+      <c r="F20" s="206"/>
       <c r="G20" s="66"/>
       <c r="H20" s="66"/>
       <c r="I20" s="66"/>
-      <c r="J20" s="96"/>
-    </row>
-    <row r="21" spans="3:10">
-      <c r="C21" s="89"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="88"/>
-      <c r="J21" s="76"/>
-    </row>
-    <row r="22" spans="3:10">
-      <c r="C22" s="90"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="201" t="s">
+      <c r="J20" s="66"/>
+      <c r="K20" s="93"/>
+    </row>
+    <row r="21" spans="4:11">
+      <c r="D21" s="84"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="74"/>
+    </row>
+    <row r="22" spans="4:11">
+      <c r="D22" s="87"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="207" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="202"/>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="203"/>
-      <c r="J22" s="76"/>
-    </row>
-    <row r="23" spans="3:10">
-      <c r="C23" s="84"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="204"/>
-      <c r="F23" s="205"/>
-      <c r="G23" s="205"/>
-      <c r="H23" s="205"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="76"/>
-    </row>
-    <row r="24" spans="3:10">
-      <c r="C24" s="86"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="76"/>
-    </row>
-    <row r="25" spans="3:10">
-      <c r="C25" s="84"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="209" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="210"/>
-      <c r="G25" s="210"/>
-      <c r="H25" s="210"/>
-      <c r="I25" s="211"/>
-      <c r="J25" s="76"/>
-    </row>
-    <row r="26" spans="3:10">
-      <c r="C26" s="84"/>
-      <c r="D26" s="85"/>
-      <c r="E26" s="212"/>
-      <c r="F26" s="213"/>
-      <c r="G26" s="213"/>
-      <c r="H26" s="213"/>
-      <c r="I26" s="214"/>
-      <c r="J26" s="76"/>
-    </row>
-    <row r="27" spans="3:10">
-      <c r="C27" s="86"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="76"/>
-    </row>
-    <row r="28" spans="3:10">
-      <c r="C28" s="84"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="83"/>
-      <c r="J28" s="76"/>
-    </row>
-    <row r="29" spans="3:10">
-      <c r="C29" s="231" t="s">
+      <c r="G22" s="208"/>
+      <c r="H22" s="208"/>
+      <c r="I22" s="208"/>
+      <c r="J22" s="209"/>
+      <c r="K22" s="74"/>
+    </row>
+    <row r="23" spans="4:11">
+      <c r="D23" s="82"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="210"/>
+      <c r="G23" s="211"/>
+      <c r="H23" s="211"/>
+      <c r="I23" s="211"/>
+      <c r="J23" s="212"/>
+      <c r="K23" s="74"/>
+    </row>
+    <row r="24" spans="4:11">
+      <c r="D24" s="82"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="242"/>
+      <c r="H24" s="242"/>
+      <c r="I24" s="242"/>
+      <c r="J24" s="242"/>
+      <c r="K24" s="74"/>
+    </row>
+    <row r="25" spans="4:11">
+      <c r="D25" s="88"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="91"/>
+    </row>
+    <row r="26" spans="4:11">
+      <c r="D26" s="187" t="s">
         <v>118</v>
       </c>
-      <c r="D29" s="208"/>
-      <c r="E29" s="208"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="96"/>
-    </row>
-    <row r="30" spans="3:10">
-      <c r="C30" s="86"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="76"/>
-    </row>
-    <row r="31" spans="3:10" ht="15" customHeight="1">
-      <c r="C31" s="90"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="209" t="s">
-        <v>119</v>
-      </c>
-      <c r="G31" s="210"/>
-      <c r="H31" s="210"/>
-      <c r="I31" s="211"/>
-      <c r="J31" s="76"/>
-    </row>
-    <row r="32" spans="3:10">
-      <c r="C32" s="84"/>
-      <c r="D32" s="85"/>
-      <c r="E32" s="85"/>
-      <c r="F32" s="212"/>
-      <c r="G32" s="213"/>
-      <c r="H32" s="213"/>
-      <c r="I32" s="214"/>
-      <c r="J32" s="76"/>
-    </row>
-    <row r="33" spans="3:10">
-      <c r="C33" s="91"/>
-      <c r="D33" s="92"/>
-      <c r="E33" s="92"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="93"/>
-      <c r="H33" s="93"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="94"/>
-    </row>
-    <row r="34" spans="3:10">
-      <c r="C34" s="189" t="s">
-        <v>120</v>
-      </c>
-      <c r="D34" s="190"/>
-      <c r="E34" s="190"/>
-      <c r="F34" s="190"/>
-      <c r="G34" s="190"/>
-      <c r="H34" s="190"/>
-      <c r="I34" s="191" t="s">
+      <c r="E26" s="188"/>
+      <c r="F26" s="188"/>
+      <c r="G26" s="188"/>
+      <c r="H26" s="188"/>
+      <c r="I26" s="188"/>
+      <c r="J26" s="189" t="s">
         <v>19</v>
       </c>
-      <c r="J34" s="192"/>
-    </row>
+      <c r="K26" s="190"/>
+    </row>
+    <row r="35" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I17"/>
-    <mergeCell ref="E22:I23"/>
-    <mergeCell ref="E25:I26"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F31:I32"/>
+  <mergeCells count="19">
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="F22:J23"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:J17"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5187,11 +5107,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46F92D6-0887-4A5A-AFC7-87E289EC819A}">
   <dimension ref="D4:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -5201,7 +5121,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
@@ -5215,308 +5135,309 @@
       <c r="K4" s="45"/>
     </row>
     <row r="5" spans="4:11">
-      <c r="D5" s="232" t="s">
+      <c r="D5" s="230" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="233"/>
-      <c r="F5" s="233"/>
-      <c r="G5" s="233"/>
-      <c r="H5" s="234" t="s">
+      <c r="E5" s="231"/>
+      <c r="F5" s="231"/>
+      <c r="G5" s="231"/>
+      <c r="H5" s="232" t="s">
         <v>110</v>
       </c>
-      <c r="I5" s="234"/>
-      <c r="J5" s="234"/>
-      <c r="K5" s="235"/>
+      <c r="I5" s="232"/>
+      <c r="J5" s="232"/>
+      <c r="K5" s="233"/>
     </row>
     <row r="6" spans="4:11">
-      <c r="D6" s="184"/>
-      <c r="E6" s="185"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="75"/>
+      <c r="D6" s="182"/>
+      <c r="E6" s="183"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="73"/>
     </row>
     <row r="7" spans="4:11">
-      <c r="D7" s="182" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="76"/>
+      <c r="D7" s="181" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="243"/>
+      <c r="F7" s="243"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="74"/>
     </row>
     <row r="8" spans="4:11">
-      <c r="D8" s="77"/>
+      <c r="D8" s="75"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="35"/>
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
-      <c r="K8" s="76"/>
+      <c r="K8" s="74"/>
     </row>
     <row r="9" spans="4:11">
-      <c r="D9" s="217" t="s">
+      <c r="D9" s="215" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="218"/>
-      <c r="F9" s="218"/>
-      <c r="G9" s="186" t="s">
-        <v>123</v>
-      </c>
-      <c r="H9" s="187"/>
-      <c r="I9" s="187"/>
-      <c r="J9" s="188"/>
-      <c r="K9" s="78"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="216"/>
+      <c r="G9" s="184" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="185"/>
+      <c r="I9" s="185"/>
+      <c r="J9" s="186"/>
+      <c r="K9" s="76"/>
     </row>
     <row r="10" spans="4:11">
-      <c r="D10" s="193" t="s">
+      <c r="D10" s="191" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="116"/>
-      <c r="F10" s="116"/>
-      <c r="G10" s="176" t="s">
+      <c r="E10" s="115"/>
+      <c r="F10" s="115"/>
+      <c r="G10" s="175" t="s">
         <v>87</v>
       </c>
-      <c r="H10" s="177"/>
-      <c r="I10" s="177"/>
-      <c r="J10" s="178"/>
-      <c r="K10" s="79"/>
+      <c r="H10" s="176"/>
+      <c r="I10" s="176"/>
+      <c r="J10" s="177"/>
+      <c r="K10" s="77"/>
     </row>
     <row r="11" spans="4:11">
-      <c r="D11" s="217" t="s">
+      <c r="D11" s="215" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="183"/>
-      <c r="F11" s="183"/>
-      <c r="G11" s="222" t="s">
-        <v>124</v>
-      </c>
-      <c r="H11" s="223"/>
-      <c r="I11" s="223"/>
-      <c r="J11" s="224"/>
-      <c r="K11" s="79"/>
+      <c r="E11" s="243"/>
+      <c r="F11" s="243"/>
+      <c r="G11" s="220" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="221"/>
+      <c r="I11" s="221"/>
+      <c r="J11" s="222"/>
+      <c r="K11" s="77"/>
     </row>
     <row r="12" spans="4:11">
-      <c r="D12" s="80"/>
+      <c r="D12" s="78"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="65"/>
       <c r="H12" s="65"/>
       <c r="I12" s="65"/>
       <c r="J12" s="65"/>
-      <c r="K12" s="81"/>
+      <c r="K12" s="79"/>
     </row>
     <row r="13" spans="4:11">
-      <c r="D13" s="225" t="s">
+      <c r="D13" s="223" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="125"/>
+      <c r="H13" s="125"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="125"/>
+      <c r="K13" s="74"/>
+    </row>
+    <row r="14" spans="4:11">
+      <c r="D14" s="80"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="74"/>
+    </row>
+    <row r="15" spans="4:11" ht="15" customHeight="1">
+      <c r="D15" s="217" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="218"/>
+      <c r="F15" s="219"/>
+      <c r="G15" s="193" t="s">
         <v>125</v>
       </c>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="126"/>
-      <c r="H13" s="126"/>
-      <c r="I13" s="126"/>
-      <c r="J13" s="126"/>
-      <c r="K13" s="76"/>
-    </row>
-    <row r="14" spans="4:11">
-      <c r="D14" s="82"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="76"/>
-    </row>
-    <row r="15" spans="4:11" ht="15" customHeight="1">
-      <c r="D15" s="219" t="s">
+      <c r="H15" s="224"/>
+      <c r="I15" s="224"/>
+      <c r="J15" s="225"/>
+      <c r="K15" s="74"/>
+    </row>
+    <row r="16" spans="4:11">
+      <c r="D16" s="82"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="226"/>
+      <c r="H16" s="227"/>
+      <c r="I16" s="227"/>
+      <c r="J16" s="228"/>
+      <c r="K16" s="74"/>
+    </row>
+    <row r="17" spans="4:11">
+      <c r="D17" s="84"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="74"/>
+    </row>
+    <row r="18" spans="4:11" ht="15" customHeight="1">
+      <c r="D18" s="217" t="s">
         <v>126</v>
       </c>
-      <c r="E15" s="220"/>
-      <c r="F15" s="221"/>
-      <c r="G15" s="195" t="s">
+      <c r="E18" s="218"/>
+      <c r="F18" s="219"/>
+      <c r="G18" s="193" t="s">
         <v>127</v>
       </c>
-      <c r="H15" s="226"/>
-      <c r="I15" s="226"/>
-      <c r="J15" s="227"/>
-      <c r="K15" s="76"/>
-    </row>
-    <row r="16" spans="4:11">
-      <c r="D16" s="84"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="228"/>
-      <c r="H16" s="229"/>
-      <c r="I16" s="229"/>
-      <c r="J16" s="230"/>
-      <c r="K16" s="76"/>
-    </row>
-    <row r="17" spans="4:11">
-      <c r="D17" s="86"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="76"/>
-    </row>
-    <row r="18" spans="4:11">
-      <c r="D18" s="219" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" s="220"/>
-      <c r="F18" s="221"/>
-      <c r="G18" s="195" t="s">
-        <v>129</v>
-      </c>
-      <c r="H18" s="226"/>
-      <c r="I18" s="226"/>
-      <c r="J18" s="227"/>
-      <c r="K18" s="76"/>
+      <c r="H18" s="224"/>
+      <c r="I18" s="224"/>
+      <c r="J18" s="225"/>
+      <c r="K18" s="74"/>
     </row>
     <row r="19" spans="4:11">
-      <c r="D19" s="84"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="228"/>
-      <c r="H19" s="229"/>
-      <c r="I19" s="229"/>
-      <c r="J19" s="230"/>
-      <c r="K19" s="76"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="226"/>
+      <c r="H19" s="227"/>
+      <c r="I19" s="227"/>
+      <c r="J19" s="228"/>
+      <c r="K19" s="74"/>
     </row>
     <row r="20" spans="4:11">
-      <c r="D20" s="86"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
-      <c r="K20" s="76"/>
+      <c r="K20" s="74"/>
     </row>
     <row r="21" spans="4:11">
-      <c r="D21" s="99"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="96"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="93"/>
     </row>
     <row r="22" spans="4:11" ht="15" customHeight="1">
-      <c r="D22" s="236" t="s">
+      <c r="D22" s="234" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="218"/>
+      <c r="F22" s="218"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="81"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="74"/>
+    </row>
+    <row r="23" spans="4:11">
+      <c r="D23" s="84"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="74"/>
+    </row>
+    <row r="24" spans="4:11" ht="15" customHeight="1">
+      <c r="D24" s="238" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="218"/>
+      <c r="F24" s="219"/>
+      <c r="G24" s="207" t="s">
         <v>130</v>
       </c>
-      <c r="E22" s="220"/>
-      <c r="F22" s="220"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="83"/>
-      <c r="K22" s="76"/>
-    </row>
-    <row r="23" spans="4:11">
-      <c r="D23" s="86"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="76"/>
-    </row>
-    <row r="24" spans="4:11" ht="15" customHeight="1">
-      <c r="D24" s="240" t="s">
-        <v>131</v>
-      </c>
-      <c r="E24" s="220"/>
-      <c r="F24" s="221"/>
-      <c r="G24" s="209" t="s">
-        <v>132</v>
-      </c>
-      <c r="H24" s="210"/>
-      <c r="I24" s="210"/>
-      <c r="J24" s="211"/>
-      <c r="K24" s="76"/>
+      <c r="H24" s="208"/>
+      <c r="I24" s="208"/>
+      <c r="J24" s="209"/>
+      <c r="K24" s="74"/>
     </row>
     <row r="25" spans="4:11">
-      <c r="D25" s="84"/>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="212"/>
-      <c r="H25" s="213"/>
-      <c r="I25" s="213"/>
-      <c r="J25" s="214"/>
-      <c r="K25" s="76"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="210"/>
+      <c r="H25" s="211"/>
+      <c r="I25" s="211"/>
+      <c r="J25" s="212"/>
+      <c r="K25" s="74"/>
     </row>
     <row r="26" spans="4:11">
-      <c r="D26" s="84"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
       <c r="G26" s="35"/>
       <c r="H26" s="35"/>
       <c r="I26" s="35"/>
       <c r="J26" s="35"/>
-      <c r="K26" s="76"/>
+      <c r="K26" s="74"/>
     </row>
     <row r="27" spans="4:11" ht="15.75">
-      <c r="D27" s="237" t="s">
+      <c r="D27" s="235" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="236"/>
+      <c r="F27" s="237"/>
+      <c r="G27" s="207" t="s">
+        <v>132</v>
+      </c>
+      <c r="H27" s="208"/>
+      <c r="I27" s="208"/>
+      <c r="J27" s="209"/>
+      <c r="K27" s="74"/>
+    </row>
+    <row r="28" spans="4:11">
+      <c r="D28" s="82"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="210"/>
+      <c r="H28" s="211"/>
+      <c r="I28" s="211"/>
+      <c r="J28" s="212"/>
+      <c r="K28" s="74"/>
+    </row>
+    <row r="29" spans="4:11">
+      <c r="D29" s="88"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="91"/>
+    </row>
+    <row r="30" spans="4:11">
+      <c r="D30" s="187" t="s">
         <v>133</v>
       </c>
-      <c r="E27" s="238"/>
-      <c r="F27" s="239"/>
-      <c r="G27" s="209" t="s">
-        <v>134</v>
-      </c>
-      <c r="H27" s="210"/>
-      <c r="I27" s="210"/>
-      <c r="J27" s="211"/>
-      <c r="K27" s="76"/>
-    </row>
-    <row r="28" spans="4:11">
-      <c r="D28" s="84"/>
-      <c r="E28" s="85"/>
-      <c r="F28" s="85"/>
-      <c r="G28" s="212"/>
-      <c r="H28" s="213"/>
-      <c r="I28" s="213"/>
-      <c r="J28" s="214"/>
-      <c r="K28" s="76"/>
-    </row>
-    <row r="29" spans="4:11">
-      <c r="D29" s="91"/>
-      <c r="E29" s="92"/>
-      <c r="F29" s="92"/>
-      <c r="G29" s="93"/>
-      <c r="H29" s="93"/>
-      <c r="I29" s="93"/>
-      <c r="J29" s="93"/>
-      <c r="K29" s="94"/>
-    </row>
-    <row r="30" spans="4:11">
-      <c r="D30" s="189" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" s="190"/>
-      <c r="F30" s="190"/>
-      <c r="G30" s="190"/>
-      <c r="H30" s="190"/>
-      <c r="I30" s="190"/>
-      <c r="J30" s="191" t="s">
+      <c r="E30" s="188"/>
+      <c r="F30" s="188"/>
+      <c r="G30" s="188"/>
+      <c r="H30" s="188"/>
+      <c r="I30" s="188"/>
+      <c r="J30" s="189" t="s">
         <v>19</v>
       </c>
-      <c r="K30" s="192"/>
+      <c r="K30" s="190"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G15:J16"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:J19"/>
     <mergeCell ref="D30:I30"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="G27:J28"/>
@@ -5524,23 +5445,379 @@
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="G24:J25"/>
     <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:J19"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="G7:J7"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="G10:J10"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:J11"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5103EF-7205-4AA0-90EA-46DDC5E22830}">
+  <dimension ref="C2:P32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="3:13" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:13">
+      <c r="C3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="239" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="239"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="29">
+        <v>45323</v>
+      </c>
+      <c r="J3" s="30"/>
+    </row>
+    <row r="4" spans="3:13">
+      <c r="C4" s="240" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="232" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="232"/>
+      <c r="I4" s="232"/>
+      <c r="J4" s="241"/>
+    </row>
+    <row r="5" spans="3:13">
+      <c r="C5" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="113"/>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="3:13">
+      <c r="C6" s="13"/>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="3:13">
+      <c r="C7" s="114" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="125" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="3:13">
+      <c r="C8" s="114" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="125" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="3:13">
+      <c r="C9" s="16"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="3:13">
+      <c r="C10" s="112" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="3:13">
+      <c r="C11" s="13"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="3:13">
+      <c r="C12" s="114" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="125" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="125"/>
+      <c r="H12" s="125"/>
+      <c r="I12" s="125"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="3:13">
+      <c r="C13" s="114" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="125" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="125"/>
+      <c r="H13" s="125"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="3:13">
+      <c r="C14" s="114" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="115"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="125" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="125"/>
+      <c r="H14" s="125"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="3:13" ht="15.75">
+      <c r="C15" s="16"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="17"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="3:13">
+      <c r="C16" s="112" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" s="113"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="3:16">
+      <c r="C17" s="13"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="3:16">
+      <c r="C18" s="114" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="115"/>
+      <c r="E18" s="115"/>
+      <c r="F18" s="125" t="s">
+        <v>139</v>
+      </c>
+      <c r="G18" s="125"/>
+      <c r="H18" s="125"/>
+      <c r="I18" s="125"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="3:16" ht="15" customHeight="1">
+      <c r="C19" s="13"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="107"/>
+      <c r="I19" s="107"/>
+      <c r="J19" s="106"/>
+    </row>
+    <row r="20" spans="3:16">
+      <c r="C20" s="114" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="115"/>
+      <c r="E20" s="115"/>
+      <c r="F20" s="125" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="125"/>
+      <c r="H20" s="125"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="106"/>
+    </row>
+    <row r="21" spans="3:16">
+      <c r="C21" s="13"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="3:16">
+      <c r="C22" s="114" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="115"/>
+      <c r="E22" s="115"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="3:16" ht="15" customHeight="1">
+      <c r="C23" s="13"/>
+      <c r="D23" s="126" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="127"/>
+      <c r="I23" s="127"/>
+      <c r="J23" s="128"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="3:16">
+      <c r="C24" s="13"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="130"/>
+      <c r="F24" s="130"/>
+      <c r="G24" s="130"/>
+      <c r="H24" s="130"/>
+      <c r="I24" s="130"/>
+      <c r="J24" s="131"/>
+    </row>
+    <row r="25" spans="3:16">
+      <c r="C25" s="13"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="131"/>
+    </row>
+    <row r="26" spans="3:16">
+      <c r="C26" s="13"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="130"/>
+      <c r="H26" s="130"/>
+      <c r="I26" s="130"/>
+      <c r="J26" s="131"/>
+    </row>
+    <row r="27" spans="3:16">
+      <c r="C27" s="13"/>
+      <c r="D27" s="129"/>
+      <c r="E27" s="130"/>
+      <c r="F27" s="130"/>
+      <c r="G27" s="130"/>
+      <c r="H27" s="130"/>
+      <c r="I27" s="130"/>
+      <c r="J27" s="131"/>
+    </row>
+    <row r="28" spans="3:16">
+      <c r="C28" s="13"/>
+      <c r="D28" s="129"/>
+      <c r="E28" s="130"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="130"/>
+      <c r="J28" s="131"/>
+    </row>
+    <row r="29" spans="3:16">
+      <c r="C29" s="13"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="133"/>
+      <c r="F29" s="133"/>
+      <c r="G29" s="133"/>
+      <c r="H29" s="133"/>
+      <c r="I29" s="133"/>
+      <c r="J29" s="134"/>
+    </row>
+    <row r="30" spans="3:16">
+      <c r="C30" s="13"/>
+      <c r="D30" s="105"/>
+      <c r="E30" s="105"/>
+      <c r="F30" s="105"/>
+      <c r="G30" s="105"/>
+      <c r="H30" s="105"/>
+      <c r="I30" s="105"/>
+      <c r="J30" s="104"/>
+    </row>
+    <row r="31" spans="3:16" ht="15.75" thickBot="1">
+      <c r="C31" s="18"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="20"/>
+    </row>
+    <row r="32" spans="3:16" ht="15.75" thickBot="1">
+      <c r="C32" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="109"/>
+      <c r="E32" s="109"/>
+      <c r="F32" s="109"/>
+      <c r="G32" s="109"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" s="111"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D23:J29"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:I13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Plantillas incluidas en la v3
</commit_message>
<xml_diff>
--- a/Procesos/ControlDeCambios/Plantillas.xlsx
+++ b/Procesos/ControlDeCambios/Plantillas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/roi_martinez_enriquez_rai_usc_es/Documents/GrEI/EnSo/6_GestConf/Semana2/Arquivos/Documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/roi_martinez_enriquez_rai_usc_es/Documents/GrEI/EnSo/6_GestConf/Semana3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1231" documentId="8_{510C91CE-A6A1-4AC1-8291-D918ED7F11D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F18E18A-5F73-49EB-BC74-5A7E2FD4F56B}"/>
+  <xr:revisionPtr revIDLastSave="1315" documentId="8_{510C91CE-A6A1-4AC1-8291-D918ED7F11D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4CB858D-3AA7-4DDE-98A3-8BDCA8286B3D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="7" xr2:uid="{6645DB64-4FE3-44F8-AF56-BC889C6C1641}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6645DB64-4FE3-44F8-AF56-BC889C6C1641}"/>
   </bookViews>
   <sheets>
     <sheet name="IdfSlc" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="155">
   <si>
     <t xml:space="preserve">ID: </t>
   </si>
@@ -127,6 +127,12 @@
     <t>Evaluación</t>
   </si>
   <si>
+    <t>Resolución:</t>
+  </si>
+  <si>
+    <t>[Indique si el cambio es ACEPTADO o RECHAZADO]</t>
+  </si>
+  <si>
     <t>Factibilidad técnica:</t>
   </si>
   <si>
@@ -187,12 +193,6 @@
     <t>Decisiones</t>
   </si>
   <si>
-    <t>Resolución:</t>
-  </si>
-  <si>
-    <t>[Indique si el cambio es ACEPTADO o RECHAZADO]</t>
-  </si>
-  <si>
     <t>Nivel de prioridad:</t>
   </si>
   <si>
@@ -236,6 +236,21 @@
   </si>
   <si>
     <t>[De haber, especifique las medidas de mitigación para los posibles riesgos identificados]</t>
+  </si>
+  <si>
+    <t>Poker Scrum</t>
+  </si>
+  <si>
+    <t>Tiempo Mínimo</t>
+  </si>
+  <si>
+    <t>Tiempo Máximo</t>
+  </si>
+  <si>
+    <t>Tiempo más probable</t>
+  </si>
+  <si>
+    <t>Tiempo Medio</t>
   </si>
   <si>
     <t>PLANIFICACIÓN</t>
@@ -514,6 +529,21 @@
   </si>
   <si>
     <t>NOTIFICACION DE RECHAZO</t>
+  </si>
+  <si>
+    <t>[Indique el nombre del dueño de la estimación]</t>
+  </si>
+  <si>
+    <t>[Valor y justificación de la decisión de tiempo mínimo]</t>
+  </si>
+  <si>
+    <t>[Valor y justificación de la decisión de tiempo máximo]</t>
+  </si>
+  <si>
+    <t>[Indique el valor y el número de veces que se repitió]</t>
+  </si>
+  <si>
+    <t>[Resultado de aplicar la fórmula (Tmin + 4Tprob + Tmax)/6]</t>
   </si>
 </sst>
 </file>
@@ -709,7 +739,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="84">
+  <borders count="86">
     <border>
       <left/>
       <right/>
@@ -1646,11 +1676,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
@@ -1851,6 +1903,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1861,18 +1935,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1902,8 +1964,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1932,35 +2003,44 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1986,26 +2066,50 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="59" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2031,153 +2135,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="59" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="78" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="79" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2187,6 +2144,48 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2196,6 +2195,78 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="78" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="79" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2212,9 +2283,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2253,10 +2321,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2277,7 +2342,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2576,10 +2641,10 @@
   <dimension ref="C2:P35"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="C4:J8"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="3:10" ht="15.75" thickBot="1"/>
     <row r="3" spans="3:10" ht="15.75" thickBot="1">
@@ -2601,10 +2666,10 @@
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="3:10">
-      <c r="C4" s="112" t="s">
+      <c r="C4" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="113"/>
+      <c r="D4" s="115"/>
       <c r="J4" s="14"/>
     </row>
     <row r="5" spans="3:10">
@@ -2612,31 +2677,31 @@
       <c r="J5" s="14"/>
     </row>
     <row r="6" spans="3:10">
-      <c r="C6" s="114" t="s">
+      <c r="C6" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="125" t="s">
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="125"/>
-      <c r="H6" s="125"/>
-      <c r="I6" s="125"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="114" t="s">
+      <c r="C7" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="125" t="s">
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="3:10">
@@ -2650,10 +2715,10 @@
       <c r="J8" s="17"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="112" t="s">
+      <c r="C9" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="113"/>
+      <c r="D9" s="115"/>
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="3:10">
@@ -2661,108 +2726,108 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="3:10">
-      <c r="C11" s="114" t="s">
+      <c r="C11" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="115"/>
-      <c r="E11" s="115"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="113"/>
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="3:10">
       <c r="C12" s="13"/>
-      <c r="D12" s="116" t="s">
+      <c r="D12" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
-      <c r="G12" s="117"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="117"/>
-      <c r="J12" s="118"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="121"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="122"/>
     </row>
     <row r="13" spans="3:10">
       <c r="C13" s="13"/>
-      <c r="D13" s="119"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="121"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="124"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="125"/>
     </row>
     <row r="14" spans="3:10">
       <c r="C14" s="13"/>
-      <c r="D14" s="122"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="123"/>
-      <c r="H14" s="123"/>
-      <c r="I14" s="123"/>
-      <c r="J14" s="124"/>
+      <c r="D14" s="126"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="128"/>
     </row>
     <row r="15" spans="3:10">
       <c r="C15" s="13"/>
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="3:10">
-      <c r="C16" s="114" t="s">
+      <c r="C16" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="115"/>
-      <c r="E16" s="115"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="113"/>
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="3:16">
       <c r="C17" s="13"/>
-      <c r="D17" s="116" t="s">
+      <c r="D17" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="117"/>
-      <c r="H17" s="117"/>
-      <c r="I17" s="117"/>
-      <c r="J17" s="118"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="121"/>
+      <c r="H17" s="121"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="122"/>
     </row>
     <row r="18" spans="3:16">
       <c r="C18" s="13"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="120"/>
-      <c r="J18" s="121"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="124"/>
+      <c r="H18" s="124"/>
+      <c r="I18" s="124"/>
+      <c r="J18" s="125"/>
     </row>
     <row r="19" spans="3:16">
       <c r="C19" s="13"/>
-      <c r="D19" s="119"/>
-      <c r="E19" s="120"/>
-      <c r="F19" s="120"/>
-      <c r="G19" s="120"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="120"/>
-      <c r="J19" s="121"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="125"/>
     </row>
     <row r="20" spans="3:16">
       <c r="C20" s="13"/>
-      <c r="D20" s="119"/>
-      <c r="E20" s="120"/>
-      <c r="F20" s="120"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="120"/>
-      <c r="I20" s="120"/>
-      <c r="J20" s="121"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="124"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="124"/>
+      <c r="H20" s="124"/>
+      <c r="I20" s="124"/>
+      <c r="J20" s="125"/>
     </row>
     <row r="21" spans="3:16">
       <c r="C21" s="13"/>
-      <c r="D21" s="122"/>
-      <c r="E21" s="123"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="123"/>
-      <c r="H21" s="123"/>
-      <c r="I21" s="123"/>
-      <c r="J21" s="124"/>
+      <c r="D21" s="126"/>
+      <c r="E21" s="127"/>
+      <c r="F21" s="127"/>
+      <c r="G21" s="127"/>
+      <c r="H21" s="127"/>
+      <c r="I21" s="127"/>
+      <c r="J21" s="128"/>
     </row>
     <row r="22" spans="3:16">
       <c r="C22" s="16"/>
@@ -2775,10 +2840,10 @@
       <c r="J22" s="17"/>
     </row>
     <row r="23" spans="3:16">
-      <c r="C23" s="112" t="s">
+      <c r="C23" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="113"/>
+      <c r="D23" s="115"/>
       <c r="J23" s="14"/>
     </row>
     <row r="24" spans="3:16">
@@ -2786,89 +2851,89 @@
       <c r="J24" s="14"/>
     </row>
     <row r="25" spans="3:16">
-      <c r="C25" s="114" t="s">
+      <c r="C25" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="115"/>
-      <c r="E25" s="115"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="113"/>
       <c r="J25" s="14"/>
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="3:16">
       <c r="C26" s="13"/>
-      <c r="D26" s="116" t="s">
+      <c r="D26" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="117"/>
-      <c r="F26" s="117"/>
-      <c r="G26" s="117"/>
-      <c r="H26" s="117"/>
-      <c r="I26" s="117"/>
-      <c r="J26" s="118"/>
+      <c r="E26" s="121"/>
+      <c r="F26" s="121"/>
+      <c r="G26" s="121"/>
+      <c r="H26" s="121"/>
+      <c r="I26" s="121"/>
+      <c r="J26" s="122"/>
     </row>
     <row r="27" spans="3:16">
       <c r="C27" s="13"/>
-      <c r="D27" s="119"/>
-      <c r="E27" s="120"/>
-      <c r="F27" s="120"/>
-      <c r="G27" s="120"/>
-      <c r="H27" s="120"/>
-      <c r="I27" s="120"/>
-      <c r="J27" s="121"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="124"/>
+      <c r="G27" s="124"/>
+      <c r="H27" s="124"/>
+      <c r="I27" s="124"/>
+      <c r="J27" s="125"/>
     </row>
     <row r="28" spans="3:16">
       <c r="C28" s="13"/>
-      <c r="D28" s="122"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="123"/>
-      <c r="G28" s="123"/>
-      <c r="H28" s="123"/>
-      <c r="I28" s="123"/>
-      <c r="J28" s="124"/>
+      <c r="D28" s="126"/>
+      <c r="E28" s="127"/>
+      <c r="F28" s="127"/>
+      <c r="G28" s="127"/>
+      <c r="H28" s="127"/>
+      <c r="I28" s="127"/>
+      <c r="J28" s="128"/>
     </row>
     <row r="29" spans="3:16">
       <c r="C29" s="13"/>
       <c r="J29" s="14"/>
     </row>
     <row r="30" spans="3:16">
-      <c r="C30" s="114" t="s">
+      <c r="C30" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="115"/>
-      <c r="E30" s="115"/>
+      <c r="D30" s="113"/>
+      <c r="E30" s="113"/>
       <c r="J30" s="14"/>
     </row>
     <row r="31" spans="3:16">
       <c r="C31" s="13"/>
-      <c r="D31" s="116" t="s">
+      <c r="D31" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="117"/>
-      <c r="F31" s="117"/>
-      <c r="G31" s="117"/>
-      <c r="H31" s="117"/>
-      <c r="I31" s="117"/>
-      <c r="J31" s="118"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="121"/>
+      <c r="G31" s="121"/>
+      <c r="H31" s="121"/>
+      <c r="I31" s="121"/>
+      <c r="J31" s="122"/>
     </row>
     <row r="32" spans="3:16">
       <c r="C32" s="13"/>
-      <c r="D32" s="119"/>
-      <c r="E32" s="120"/>
-      <c r="F32" s="120"/>
-      <c r="G32" s="120"/>
-      <c r="H32" s="120"/>
-      <c r="I32" s="120"/>
-      <c r="J32" s="121"/>
+      <c r="D32" s="123"/>
+      <c r="E32" s="124"/>
+      <c r="F32" s="124"/>
+      <c r="G32" s="124"/>
+      <c r="H32" s="124"/>
+      <c r="I32" s="124"/>
+      <c r="J32" s="125"/>
     </row>
     <row r="33" spans="3:10">
       <c r="C33" s="13"/>
-      <c r="D33" s="122"/>
-      <c r="E33" s="123"/>
-      <c r="F33" s="123"/>
-      <c r="G33" s="123"/>
-      <c r="H33" s="123"/>
-      <c r="I33" s="123"/>
-      <c r="J33" s="124"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="127"/>
+      <c r="F33" s="127"/>
+      <c r="G33" s="127"/>
+      <c r="H33" s="127"/>
+      <c r="I33" s="127"/>
+      <c r="J33" s="128"/>
     </row>
     <row r="34" spans="3:10" ht="15.75" thickBot="1">
       <c r="C34" s="18"/>
@@ -2881,26 +2946,21 @@
       <c r="J34" s="20"/>
     </row>
     <row r="35" spans="3:10" ht="15.75" thickBot="1">
-      <c r="C35" s="108" t="s">
+      <c r="C35" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="109"/>
-      <c r="E35" s="109"/>
-      <c r="F35" s="109"/>
-      <c r="G35" s="109"/>
-      <c r="H35" s="109"/>
-      <c r="I35" s="110" t="s">
+      <c r="D35" s="117"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="117"/>
+      <c r="H35" s="117"/>
+      <c r="I35" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="111"/>
+      <c r="J35" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C7:E7"/>
     <mergeCell ref="C35:H35"/>
     <mergeCell ref="I35:J35"/>
     <mergeCell ref="C9:D9"/>
@@ -2913,6 +2973,11 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2921,13 +2986,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7651F806-68F4-4E68-A906-F21ED235D482}">
-  <dimension ref="C2:P32"/>
+  <dimension ref="C2:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="3:13" ht="15.75" thickBot="1"/>
     <row r="3" spans="3:13">
@@ -2949,24 +3014,24 @@
       <c r="J3" s="30"/>
     </row>
     <row r="4" spans="3:13">
-      <c r="C4" s="135" t="s">
+      <c r="C4" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="137" t="s">
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="137"/>
-      <c r="I4" s="137"/>
-      <c r="J4" s="138"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="132"/>
     </row>
     <row r="5" spans="3:13">
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="113"/>
+      <c r="D5" s="115"/>
       <c r="J5" s="14"/>
     </row>
     <row r="6" spans="3:13">
@@ -2974,45 +3039,45 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="3:13">
-      <c r="C7" s="114" t="s">
+      <c r="C7" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="125" t="s">
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="3:13">
-      <c r="C8" s="114" t="s">
+      <c r="C8" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="115"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="125" t="s">
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="3:13">
-      <c r="C9" s="114" t="s">
+      <c r="C9" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="115"/>
-      <c r="E9" s="115"/>
-      <c r="F9" s="125" t="s">
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="125"/>
-      <c r="H9" s="125"/>
-      <c r="I9" s="125"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="3:13" ht="15.75">
@@ -3027,218 +3092,239 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="3:13">
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="113"/>
+      <c r="D11" s="115"/>
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="3:13">
-      <c r="C12" s="13"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="109"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="3:13">
-      <c r="C13" s="114" t="s">
+      <c r="C13" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="143" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="144"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="145"/>
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="3:13">
       <c r="C14" s="13"/>
-      <c r="D14" s="126" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="127"/>
-      <c r="F14" s="127"/>
-      <c r="G14" s="127"/>
-      <c r="H14" s="127"/>
-      <c r="I14" s="127"/>
-      <c r="J14" s="128"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" spans="3:13">
-      <c r="C15" s="13"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="130"/>
-      <c r="F15" s="130"/>
-      <c r="G15" s="130"/>
-      <c r="H15" s="130"/>
-      <c r="I15" s="130"/>
-      <c r="J15" s="131"/>
+      <c r="C15" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="3:13">
       <c r="C16" s="13"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="133"/>
-      <c r="F16" s="133"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="133"/>
-      <c r="I16" s="133"/>
-      <c r="J16" s="134"/>
+      <c r="D16" s="133" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="134"/>
+      <c r="F16" s="134"/>
+      <c r="G16" s="134"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="134"/>
+      <c r="J16" s="135"/>
     </row>
     <row r="17" spans="3:16">
       <c r="C17" s="13"/>
-      <c r="J17" s="14"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="137"/>
+      <c r="F17" s="137"/>
+      <c r="G17" s="137"/>
+      <c r="H17" s="137"/>
+      <c r="I17" s="137"/>
+      <c r="J17" s="138"/>
     </row>
     <row r="18" spans="3:16">
-      <c r="C18" s="114" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="115"/>
-      <c r="E18" s="115"/>
-      <c r="J18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="140"/>
+      <c r="F18" s="140"/>
+      <c r="G18" s="140"/>
+      <c r="H18" s="140"/>
+      <c r="I18" s="140"/>
+      <c r="J18" s="141"/>
     </row>
     <row r="19" spans="3:16">
       <c r="C19" s="13"/>
-      <c r="D19" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="33"/>
+      <c r="J19" s="14"/>
     </row>
     <row r="20" spans="3:16">
-      <c r="C20" s="13"/>
+      <c r="C20" s="112" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="113"/>
+      <c r="E20" s="113"/>
       <c r="J20" s="14"/>
     </row>
     <row r="21" spans="3:16">
-      <c r="C21" s="114" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="115"/>
-      <c r="E21" s="115"/>
-      <c r="J21" s="14"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="33"/>
     </row>
     <row r="22" spans="3:16">
       <c r="C22" s="13"/>
-      <c r="D22" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="12"/>
+      <c r="J22" s="14"/>
     </row>
     <row r="23" spans="3:16">
-      <c r="C23" s="13"/>
-      <c r="D23" s="6"/>
+      <c r="C23" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
       <c r="J23" s="14"/>
     </row>
     <row r="24" spans="3:16">
       <c r="C24" s="13"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="17"/>
+      <c r="D24" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="12"/>
     </row>
     <row r="25" spans="3:16">
       <c r="C25" s="13"/>
+      <c r="D25" s="6"/>
       <c r="J25" s="14"/>
     </row>
     <row r="26" spans="3:16">
-      <c r="C26" s="114" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="115"/>
-      <c r="E26" s="115"/>
-      <c r="J26" s="14"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="3:16">
       <c r="C27" s="13"/>
-      <c r="D27" s="126" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="127"/>
-      <c r="F27" s="127"/>
-      <c r="G27" s="127"/>
-      <c r="H27" s="127"/>
-      <c r="I27" s="127"/>
-      <c r="J27" s="128"/>
-      <c r="P27" s="2"/>
+      <c r="J27" s="14"/>
     </row>
     <row r="28" spans="3:16">
-      <c r="C28" s="13"/>
-      <c r="D28" s="129"/>
-      <c r="E28" s="130"/>
-      <c r="F28" s="130"/>
-      <c r="G28" s="130"/>
-      <c r="H28" s="130"/>
-      <c r="I28" s="130"/>
-      <c r="J28" s="131"/>
+      <c r="C28" s="112" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
+      <c r="J28" s="14"/>
     </row>
     <row r="29" spans="3:16">
       <c r="C29" s="13"/>
-      <c r="D29" s="129"/>
-      <c r="E29" s="130"/>
-      <c r="F29" s="130"/>
-      <c r="G29" s="130"/>
-      <c r="H29" s="130"/>
-      <c r="I29" s="130"/>
-      <c r="J29" s="131"/>
+      <c r="D29" s="133" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="134"/>
+      <c r="F29" s="134"/>
+      <c r="G29" s="134"/>
+      <c r="H29" s="134"/>
+      <c r="I29" s="134"/>
+      <c r="J29" s="135"/>
+      <c r="P29" s="2"/>
     </row>
     <row r="30" spans="3:16">
       <c r="C30" s="13"/>
-      <c r="D30" s="132"/>
-      <c r="E30" s="133"/>
-      <c r="F30" s="133"/>
-      <c r="G30" s="133"/>
-      <c r="H30" s="133"/>
-      <c r="I30" s="133"/>
-      <c r="J30" s="134"/>
-    </row>
-    <row r="31" spans="3:16" ht="15.75" thickBot="1">
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="20"/>
-    </row>
-    <row r="32" spans="3:16" ht="15.75" thickBot="1">
-      <c r="C32" s="108" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="109"/>
-      <c r="E32" s="109"/>
-      <c r="F32" s="109"/>
-      <c r="G32" s="109"/>
-      <c r="H32" s="109"/>
-      <c r="I32" s="110" t="s">
+      <c r="D30" s="136"/>
+      <c r="E30" s="137"/>
+      <c r="F30" s="137"/>
+      <c r="G30" s="137"/>
+      <c r="H30" s="137"/>
+      <c r="I30" s="137"/>
+      <c r="J30" s="138"/>
+    </row>
+    <row r="31" spans="3:16">
+      <c r="C31" s="13"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="137"/>
+      <c r="F31" s="137"/>
+      <c r="G31" s="137"/>
+      <c r="H31" s="137"/>
+      <c r="I31" s="137"/>
+      <c r="J31" s="138"/>
+    </row>
+    <row r="32" spans="3:16">
+      <c r="C32" s="13"/>
+      <c r="D32" s="139"/>
+      <c r="E32" s="140"/>
+      <c r="F32" s="140"/>
+      <c r="G32" s="140"/>
+      <c r="H32" s="140"/>
+      <c r="I32" s="140"/>
+      <c r="J32" s="141"/>
+    </row>
+    <row r="33" spans="3:10" ht="15.75" thickBot="1">
+      <c r="C33" s="18"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="20"/>
+    </row>
+    <row r="34" spans="3:10" ht="15.75" thickBot="1">
+      <c r="C34" s="116" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="117"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="117"/>
+      <c r="H34" s="117"/>
+      <c r="I34" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="J32" s="111"/>
+      <c r="J34" s="119"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="D29:J32"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C34:H34"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="F8:I8"/>
-    <mergeCell ref="D14:J16"/>
-    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="D16:J18"/>
+    <mergeCell ref="C15:E15"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="D27:J30"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3250,10 +3336,10 @@
   <dimension ref="C2:P31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="3:13" ht="15.75" thickBot="1"/>
     <row r="3" spans="3:13">
@@ -3261,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -3275,24 +3361,24 @@
       <c r="J3" s="30"/>
     </row>
     <row r="4" spans="3:13">
-      <c r="C4" s="135" t="s">
+      <c r="C4" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="137" t="s">
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="137"/>
-      <c r="I4" s="137"/>
-      <c r="J4" s="138"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="132"/>
     </row>
     <row r="5" spans="3:13">
-      <c r="C5" s="112" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="113"/>
+      <c r="C5" s="114" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="115"/>
       <c r="J5" s="14"/>
     </row>
     <row r="6" spans="3:13">
@@ -3300,59 +3386,59 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="3:13">
-      <c r="C7" s="114" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="125" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
+      <c r="C7" s="112" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="111" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="3:13">
-      <c r="C8" s="114" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="115"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="125" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
+      <c r="C8" s="112" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="111" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="3:13">
-      <c r="C9" s="114" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="115"/>
-      <c r="E9" s="115"/>
-      <c r="F9" s="125" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="125"/>
-      <c r="H9" s="125"/>
-      <c r="I9" s="125"/>
+      <c r="C9" s="112" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="111" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="3:13">
-      <c r="C10" s="114" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="139" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="139"/>
-      <c r="H10" s="139"/>
-      <c r="I10" s="139"/>
+      <c r="C10" s="112" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="146" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="146"/>
+      <c r="H10" s="146"/>
+      <c r="I10" s="146"/>
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="3:13" ht="15.75">
@@ -3367,10 +3453,10 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="3:13">
-      <c r="C12" s="112" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="113"/>
+      <c r="C12" s="114" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="115"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="3:13">
@@ -3378,17 +3464,17 @@
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="3:13">
-      <c r="C14" s="114" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="115"/>
-      <c r="E14" s="143"/>
-      <c r="F14" s="140" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="141"/>
-      <c r="H14" s="141"/>
-      <c r="I14" s="142"/>
+      <c r="C14" s="112" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="113"/>
+      <c r="E14" s="142"/>
+      <c r="F14" s="143" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="144"/>
+      <c r="H14" s="144"/>
+      <c r="I14" s="145"/>
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="3:13">
@@ -3398,17 +3484,17 @@
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="3:13">
-      <c r="C16" s="114" t="s">
+      <c r="C16" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="115"/>
-      <c r="E16" s="143"/>
-      <c r="F16" s="140" t="s">
+      <c r="D16" s="113"/>
+      <c r="E16" s="142"/>
+      <c r="F16" s="143" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="141"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="142"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="145"/>
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="3:16">
@@ -3422,54 +3508,54 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="3:16" ht="15" customHeight="1">
-      <c r="C18" s="114" t="s">
+      <c r="C18" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="115"/>
-      <c r="E18" s="115"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="3:16">
       <c r="C19" s="13"/>
-      <c r="D19" s="126" t="s">
+      <c r="D19" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="127"/>
-      <c r="F19" s="127"/>
-      <c r="G19" s="127"/>
-      <c r="H19" s="127"/>
-      <c r="I19" s="127"/>
-      <c r="J19" s="128"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="134"/>
+      <c r="G19" s="134"/>
+      <c r="H19" s="134"/>
+      <c r="I19" s="134"/>
+      <c r="J19" s="135"/>
     </row>
     <row r="20" spans="3:16">
       <c r="C20" s="13"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="130"/>
-      <c r="F20" s="130"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="130"/>
-      <c r="I20" s="130"/>
-      <c r="J20" s="131"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="137"/>
+      <c r="F20" s="137"/>
+      <c r="G20" s="137"/>
+      <c r="H20" s="137"/>
+      <c r="I20" s="137"/>
+      <c r="J20" s="138"/>
     </row>
     <row r="21" spans="3:16">
       <c r="C21" s="13"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="130"/>
-      <c r="G21" s="130"/>
-      <c r="H21" s="130"/>
-      <c r="I21" s="130"/>
-      <c r="J21" s="131"/>
+      <c r="D21" s="136"/>
+      <c r="E21" s="137"/>
+      <c r="F21" s="137"/>
+      <c r="G21" s="137"/>
+      <c r="H21" s="137"/>
+      <c r="I21" s="137"/>
+      <c r="J21" s="138"/>
     </row>
     <row r="22" spans="3:16">
       <c r="C22" s="13"/>
-      <c r="D22" s="132"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="133"/>
-      <c r="H22" s="133"/>
-      <c r="I22" s="133"/>
-      <c r="J22" s="134"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="140"/>
+      <c r="F22" s="140"/>
+      <c r="G22" s="140"/>
+      <c r="H22" s="140"/>
+      <c r="I22" s="140"/>
+      <c r="J22" s="141"/>
     </row>
     <row r="23" spans="3:16" ht="15.75" thickBot="1">
       <c r="C23" s="18"/>
@@ -3482,24 +3568,34 @@
       <c r="J23" s="20"/>
     </row>
     <row r="24" spans="3:16" ht="15.75" thickBot="1">
-      <c r="C24" s="108" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="110" t="s">
+      <c r="C24" s="116" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="117"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="117"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="111"/>
+      <c r="J24" s="119"/>
     </row>
     <row r="31" spans="3:16">
       <c r="P31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D19:J22"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C18:E18"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="C12:D12"/>
@@ -3510,16 +3606,6 @@
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="F8:I8"/>
-    <mergeCell ref="D19:J22"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3528,13 +3614,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F72E62-C921-44D2-8B61-529931468245}">
-  <dimension ref="C3:P30"/>
+  <dimension ref="C3:P46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:I16"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37:I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="3:13">
       <c r="C3" s="40" t="s">
@@ -3555,24 +3641,24 @@
       <c r="J3" s="45"/>
     </row>
     <row r="4" spans="3:13">
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="137" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="137"/>
-      <c r="I4" s="137"/>
-      <c r="J4" s="159"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="131" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="149"/>
     </row>
     <row r="5" spans="3:13">
-      <c r="C5" s="154" t="s">
+      <c r="C5" s="150" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="113"/>
+      <c r="D5" s="115"/>
       <c r="J5" s="46"/>
     </row>
     <row r="6" spans="3:13">
@@ -3580,45 +3666,45 @@
       <c r="J6" s="46"/>
     </row>
     <row r="7" spans="3:13">
-      <c r="C7" s="144" t="s">
+      <c r="C7" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="125" t="s">
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
       <c r="J7" s="46"/>
     </row>
     <row r="8" spans="3:13">
-      <c r="C8" s="144" t="s">
+      <c r="C8" s="147" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="115"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="125" t="s">
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
       <c r="J8" s="46"/>
     </row>
     <row r="9" spans="3:13">
-      <c r="C9" s="144" t="s">
+      <c r="C9" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="115"/>
-      <c r="E9" s="115"/>
-      <c r="F9" s="153" t="s">
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="151" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="139"/>
-      <c r="H9" s="139"/>
-      <c r="I9" s="139"/>
+      <c r="G9" s="146"/>
+      <c r="H9" s="146"/>
+      <c r="I9" s="146"/>
       <c r="J9" s="46"/>
     </row>
     <row r="10" spans="3:13" ht="15.75">
@@ -3633,10 +3719,10 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="3:13">
-      <c r="C11" s="154" t="s">
+      <c r="C11" s="150" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="113"/>
+      <c r="D11" s="115"/>
       <c r="J11" s="46"/>
     </row>
     <row r="12" spans="3:13">
@@ -3644,27 +3730,27 @@
       <c r="J12" s="46"/>
     </row>
     <row r="13" spans="3:13">
-      <c r="C13" s="144" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="115"/>
-      <c r="E13" s="155"/>
-      <c r="F13" s="156" t="s">
+      <c r="C13" s="147" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="113"/>
+      <c r="E13" s="152"/>
+      <c r="F13" s="153" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="157"/>
-      <c r="H13" s="157"/>
-      <c r="I13" s="157"/>
+      <c r="G13" s="154"/>
+      <c r="H13" s="154"/>
+      <c r="I13" s="154"/>
       <c r="J13" s="60"/>
     </row>
     <row r="14" spans="3:13">
       <c r="C14" s="48"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="157"/>
-      <c r="G14" s="157"/>
-      <c r="H14" s="157"/>
-      <c r="I14" s="157"/>
+      <c r="F14" s="154"/>
+      <c r="G14" s="154"/>
+      <c r="H14" s="154"/>
+      <c r="I14" s="154"/>
       <c r="J14" s="60"/>
     </row>
     <row r="15" spans="3:13">
@@ -3674,20 +3760,20 @@
       <c r="J15" s="46"/>
     </row>
     <row r="16" spans="3:13">
-      <c r="C16" s="144" t="s">
+      <c r="C16" s="147" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="115"/>
-      <c r="E16" s="143"/>
-      <c r="F16" s="140" t="s">
+      <c r="D16" s="113"/>
+      <c r="E16" s="142"/>
+      <c r="F16" s="143" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="141"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="142"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="145"/>
       <c r="J16" s="46"/>
     </row>
-    <row r="17" spans="3:16">
+    <row r="17" spans="3:12">
       <c r="C17" s="48"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -3697,21 +3783,21 @@
       <c r="I17" s="7"/>
       <c r="J17" s="46"/>
     </row>
-    <row r="18" spans="3:16">
+    <row r="18" spans="3:12">
       <c r="C18" s="48"/>
       <c r="D18" s="10" t="s">
         <v>60</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="149" t="s">
+      <c r="F18" s="159" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="150"/>
-      <c r="H18" s="150"/>
-      <c r="I18" s="151"/>
+      <c r="G18" s="160"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="161"/>
       <c r="J18" s="46"/>
     </row>
-    <row r="19" spans="3:16">
+    <row r="19" spans="3:12">
       <c r="C19" s="48"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -3721,66 +3807,260 @@
       <c r="I19" s="7"/>
       <c r="J19" s="54"/>
     </row>
-    <row r="20" spans="3:16">
+    <row r="20" spans="3:12">
       <c r="C20" s="48"/>
       <c r="D20" s="10" t="s">
         <v>62</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="152" t="s">
+      <c r="F20" s="162" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="152"/>
-      <c r="H20" s="152"/>
-      <c r="I20" s="152"/>
+      <c r="G20" s="162"/>
+      <c r="H20" s="162"/>
+      <c r="I20" s="162"/>
       <c r="J20" s="55"/>
       <c r="L20" s="37"/>
     </row>
-    <row r="21" spans="3:16">
+    <row r="21" spans="3:12">
       <c r="C21" s="48"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="152"/>
-      <c r="G21" s="152"/>
-      <c r="H21" s="152"/>
-      <c r="I21" s="152"/>
+      <c r="F21" s="162"/>
+      <c r="G21" s="162"/>
+      <c r="H21" s="162"/>
+      <c r="I21" s="162"/>
       <c r="J21" s="61"/>
       <c r="L21" s="39"/>
     </row>
-    <row r="22" spans="3:16">
-      <c r="C22" s="56"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="57"/>
+    <row r="22" spans="3:12">
+      <c r="C22" s="47"/>
+      <c r="J22" s="46"/>
       <c r="L22" s="39"/>
     </row>
-    <row r="23" spans="3:16">
-      <c r="C23" s="145" t="s">
+    <row r="23" spans="3:12">
+      <c r="C23" s="163" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="146"/>
-      <c r="E23" s="146"/>
-      <c r="F23" s="146"/>
-      <c r="G23" s="146"/>
-      <c r="H23" s="146"/>
-      <c r="I23" s="147" t="s">
+      <c r="D23" s="164"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="92"/>
+      <c r="J23" s="110"/>
+      <c r="L23" s="39"/>
+    </row>
+    <row r="24" spans="3:12">
+      <c r="C24" s="47"/>
+      <c r="J24" s="46"/>
+      <c r="L24" s="39"/>
+    </row>
+    <row r="25" spans="3:12">
+      <c r="C25" s="147" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="113"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="159" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="160"/>
+      <c r="H25" s="160"/>
+      <c r="I25" s="161"/>
+      <c r="J25" s="46"/>
+      <c r="L25" s="39"/>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="C26" s="48"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="248"/>
+      <c r="G26" s="248"/>
+      <c r="H26" s="248"/>
+      <c r="I26" s="248"/>
+      <c r="J26" s="46"/>
+      <c r="L26" s="39"/>
+    </row>
+    <row r="27" spans="3:12">
+      <c r="C27" s="48"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="159" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="160"/>
+      <c r="H27" s="160"/>
+      <c r="I27" s="161"/>
+      <c r="J27" s="46"/>
+      <c r="L27" s="39"/>
+    </row>
+    <row r="28" spans="3:12">
+      <c r="C28" s="48"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="248"/>
+      <c r="G28" s="248"/>
+      <c r="H28" s="248"/>
+      <c r="I28" s="248"/>
+      <c r="J28" s="46"/>
+      <c r="L28" s="39"/>
+    </row>
+    <row r="29" spans="3:12">
+      <c r="C29" s="48"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="J29" s="46"/>
+      <c r="L29" s="39"/>
+    </row>
+    <row r="30" spans="3:12">
+      <c r="C30" s="147" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="113"/>
+      <c r="E30" s="113"/>
+      <c r="F30" s="159" t="s">
+        <v>150</v>
+      </c>
+      <c r="G30" s="160"/>
+      <c r="H30" s="160"/>
+      <c r="I30" s="161"/>
+      <c r="J30" s="46"/>
+      <c r="L30" s="39"/>
+    </row>
+    <row r="31" spans="3:12">
+      <c r="C31" s="48"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="248"/>
+      <c r="G31" s="248"/>
+      <c r="H31" s="248"/>
+      <c r="I31" s="248"/>
+      <c r="J31" s="46"/>
+      <c r="L31" s="39"/>
+    </row>
+    <row r="32" spans="3:12">
+      <c r="C32" s="48"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="159" t="s">
+        <v>152</v>
+      </c>
+      <c r="G32" s="160"/>
+      <c r="H32" s="160"/>
+      <c r="I32" s="161"/>
+      <c r="J32" s="46"/>
+      <c r="L32" s="39"/>
+    </row>
+    <row r="33" spans="3:16">
+      <c r="C33" s="48"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="248"/>
+      <c r="G33" s="248"/>
+      <c r="H33" s="248"/>
+      <c r="I33" s="248"/>
+      <c r="J33" s="46"/>
+      <c r="L33" s="39"/>
+    </row>
+    <row r="34" spans="3:16">
+      <c r="C34" s="47"/>
+      <c r="J34" s="46"/>
+      <c r="L34" s="39"/>
+    </row>
+    <row r="35" spans="3:16">
+      <c r="C35" s="147" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="113"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="159" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" s="160"/>
+      <c r="H35" s="160"/>
+      <c r="I35" s="161"/>
+      <c r="J35" s="46"/>
+      <c r="L35" s="39"/>
+    </row>
+    <row r="36" spans="3:16">
+      <c r="C36" s="48"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="J36" s="46"/>
+      <c r="L36" s="39"/>
+    </row>
+    <row r="37" spans="3:16">
+      <c r="C37" s="147" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="113"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="159" t="s">
+        <v>154</v>
+      </c>
+      <c r="G37" s="160"/>
+      <c r="H37" s="160"/>
+      <c r="I37" s="161"/>
+      <c r="J37" s="46"/>
+      <c r="L37" s="39"/>
+    </row>
+    <row r="38" spans="3:16">
+      <c r="C38" s="56"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="57"/>
+      <c r="L38" s="39"/>
+    </row>
+    <row r="39" spans="3:16">
+      <c r="C39" s="155" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="156"/>
+      <c r="E39" s="156"/>
+      <c r="F39" s="156"/>
+      <c r="G39" s="156"/>
+      <c r="H39" s="156"/>
+      <c r="I39" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="148"/>
-      <c r="L23" s="39"/>
-    </row>
-    <row r="24" spans="3:16">
-      <c r="L24" s="59"/>
-    </row>
-    <row r="30" spans="3:16">
-      <c r="P30" s="2"/>
+      <c r="J39" s="158"/>
+      <c r="L39" s="39"/>
+    </row>
+    <row r="40" spans="3:16">
+      <c r="L40" s="59"/>
+    </row>
+    <row r="46" spans="3:16">
+      <c r="P46" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="29">
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F20:I21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:I14"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="C4:F4"/>
@@ -3788,17 +4068,6 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:I7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:I14"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F20:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3810,17 +4079,17 @@
   <dimension ref="C3:P40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="3:10">
       <c r="C3" s="40" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
@@ -3834,24 +4103,24 @@
       <c r="J3" s="45"/>
     </row>
     <row r="4" spans="3:10">
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="137" t="s">
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="131" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="137"/>
-      <c r="I4" s="137"/>
-      <c r="J4" s="159"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="149"/>
     </row>
     <row r="5" spans="3:10">
-      <c r="C5" s="169" t="s">
+      <c r="C5" s="166" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="170"/>
+      <c r="D5" s="167"/>
       <c r="J5" s="46"/>
     </row>
     <row r="6" spans="3:10">
@@ -3859,45 +4128,45 @@
       <c r="J6" s="46"/>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="144" t="s">
+      <c r="C7" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="125" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="111" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
       <c r="J7" s="46"/>
     </row>
     <row r="8" spans="3:10">
-      <c r="C8" s="144" t="s">
+      <c r="C8" s="147" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="115"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="125" t="s">
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
       <c r="J8" s="46"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="144" t="s">
+      <c r="C9" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="115"/>
-      <c r="E9" s="115"/>
-      <c r="F9" s="153" t="s">
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="151" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="153"/>
-      <c r="H9" s="153"/>
-      <c r="I9" s="153"/>
+      <c r="G9" s="151"/>
+      <c r="H9" s="151"/>
+      <c r="I9" s="151"/>
       <c r="J9" s="46"/>
     </row>
     <row r="10" spans="3:10">
@@ -3911,10 +4180,10 @@
       <c r="J10" s="46"/>
     </row>
     <row r="11" spans="3:10">
-      <c r="C11" s="154" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="113"/>
+      <c r="C11" s="150" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="115"/>
       <c r="E11" s="10"/>
       <c r="F11" s="35"/>
       <c r="G11" s="34"/>
@@ -3935,57 +4204,57 @@
     <row r="13" spans="3:10">
       <c r="C13" s="48"/>
       <c r="D13" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E13" s="35"/>
-      <c r="F13" s="175" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="176"/>
-      <c r="H13" s="176"/>
-      <c r="I13" s="177"/>
+      <c r="F13" s="172" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="174"/>
       <c r="J13" s="49"/>
     </row>
     <row r="14" spans="3:10">
       <c r="C14" s="48"/>
       <c r="D14" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E14" s="36"/>
-      <c r="F14" s="175" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="176"/>
-      <c r="H14" s="176"/>
-      <c r="I14" s="177"/>
+      <c r="F14" s="172" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="174"/>
       <c r="J14" s="50"/>
     </row>
     <row r="15" spans="3:10">
       <c r="C15" s="48"/>
       <c r="D15" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E15" s="36"/>
-      <c r="F15" s="175" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="176"/>
-      <c r="H15" s="176"/>
-      <c r="I15" s="177"/>
+      <c r="F15" s="172" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="174"/>
       <c r="J15" s="50"/>
     </row>
     <row r="16" spans="3:10">
       <c r="C16" s="48"/>
       <c r="D16" s="10" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="178" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="179"/>
-      <c r="H16" s="179"/>
-      <c r="I16" s="180"/>
+      <c r="F16" s="175" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="176"/>
+      <c r="H16" s="176"/>
+      <c r="I16" s="177"/>
       <c r="J16" s="51"/>
     </row>
     <row r="17" spans="3:13" ht="15.75">
@@ -4000,10 +4269,10 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="3:13">
-      <c r="C18" s="169" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="170"/>
+      <c r="C18" s="166" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="167"/>
       <c r="J18" s="46"/>
     </row>
     <row r="19" spans="3:13">
@@ -4011,17 +4280,17 @@
       <c r="J19" s="46"/>
     </row>
     <row r="20" spans="3:13">
-      <c r="C20" s="144" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="115"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="166" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="150"/>
-      <c r="H20" s="150"/>
-      <c r="I20" s="167"/>
+      <c r="C20" s="147" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="113"/>
+      <c r="E20" s="142"/>
+      <c r="F20" s="184" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="160"/>
+      <c r="H20" s="160"/>
+      <c r="I20" s="185"/>
       <c r="J20" s="60"/>
     </row>
     <row r="21" spans="3:13">
@@ -4031,17 +4300,17 @@
       <c r="J21" s="46"/>
     </row>
     <row r="22" spans="3:13">
-      <c r="C22" s="144" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="115"/>
-      <c r="E22" s="143"/>
-      <c r="F22" s="140" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="141"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="142"/>
+      <c r="C22" s="147" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="113"/>
+      <c r="E22" s="142"/>
+      <c r="F22" s="143" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="144"/>
+      <c r="H22" s="144"/>
+      <c r="I22" s="145"/>
       <c r="J22" s="46"/>
     </row>
     <row r="23" spans="3:13">
@@ -4057,25 +4326,25 @@
     <row r="24" spans="3:13">
       <c r="C24" s="48"/>
       <c r="D24" s="10" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="F24" s="160" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="161"/>
-      <c r="H24" s="161"/>
-      <c r="I24" s="162"/>
+      <c r="F24" s="178" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="179"/>
+      <c r="H24" s="179"/>
+      <c r="I24" s="180"/>
       <c r="J24" s="46"/>
     </row>
     <row r="25" spans="3:13">
       <c r="C25" s="48"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="163"/>
-      <c r="G25" s="164"/>
-      <c r="H25" s="164"/>
-      <c r="I25" s="165"/>
+      <c r="F25" s="181"/>
+      <c r="G25" s="182"/>
+      <c r="H25" s="182"/>
+      <c r="I25" s="183"/>
       <c r="J25" s="46"/>
     </row>
     <row r="26" spans="3:13">
@@ -4089,17 +4358,17 @@
       <c r="J26" s="54"/>
     </row>
     <row r="27" spans="3:13">
-      <c r="C27" s="144" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="115"/>
-      <c r="E27" s="155"/>
-      <c r="F27" s="168" t="s">
-        <v>78</v>
-      </c>
-      <c r="G27" s="152"/>
-      <c r="H27" s="152"/>
-      <c r="I27" s="152"/>
+      <c r="C27" s="147" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="113"/>
+      <c r="E27" s="152"/>
+      <c r="F27" s="171" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="162"/>
+      <c r="H27" s="162"/>
+      <c r="I27" s="162"/>
       <c r="J27" s="55"/>
       <c r="L27" s="38"/>
     </row>
@@ -4107,10 +4376,10 @@
       <c r="C28" s="48"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="152"/>
-      <c r="G28" s="152"/>
-      <c r="H28" s="152"/>
-      <c r="I28" s="152"/>
+      <c r="F28" s="162"/>
+      <c r="G28" s="162"/>
+      <c r="H28" s="162"/>
+      <c r="I28" s="162"/>
       <c r="J28" s="46"/>
       <c r="L28" s="39"/>
     </row>
@@ -4126,17 +4395,17 @@
       <c r="L29" s="39"/>
     </row>
     <row r="30" spans="3:13" ht="13.5" customHeight="1">
-      <c r="C30" s="172" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="173"/>
-      <c r="E30" s="174"/>
-      <c r="F30" s="168" t="s">
-        <v>80</v>
-      </c>
-      <c r="G30" s="152"/>
-      <c r="H30" s="152"/>
-      <c r="I30" s="152"/>
+      <c r="C30" s="168" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="169"/>
+      <c r="E30" s="170"/>
+      <c r="F30" s="171" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="162"/>
+      <c r="H30" s="162"/>
+      <c r="I30" s="162"/>
       <c r="J30" s="46"/>
       <c r="L30" s="39"/>
     </row>
@@ -4144,10 +4413,10 @@
       <c r="C31" s="63"/>
       <c r="D31" s="62"/>
       <c r="E31" s="64"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="152"/>
-      <c r="H31" s="152"/>
-      <c r="I31" s="152"/>
+      <c r="F31" s="162"/>
+      <c r="G31" s="162"/>
+      <c r="H31" s="162"/>
+      <c r="I31" s="162"/>
       <c r="J31" s="46"/>
       <c r="L31" s="39"/>
     </row>
@@ -4163,24 +4432,35 @@
       <c r="L32" s="38"/>
     </row>
     <row r="33" spans="3:16">
-      <c r="C33" s="145" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="146"/>
-      <c r="E33" s="146"/>
-      <c r="F33" s="146"/>
-      <c r="G33" s="146"/>
-      <c r="H33" s="146"/>
-      <c r="I33" s="147" t="s">
+      <c r="C33" s="155" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="156"/>
+      <c r="E33" s="156"/>
+      <c r="F33" s="156"/>
+      <c r="G33" s="156"/>
+      <c r="H33" s="156"/>
+      <c r="I33" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="J33" s="171"/>
+      <c r="J33" s="165"/>
     </row>
     <row r="40" spans="3:16" ht="15" customHeight="1">
       <c r="P40" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F24:I25"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:I28"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
     <mergeCell ref="C33:H33"/>
     <mergeCell ref="I33:J33"/>
     <mergeCell ref="C11:D11"/>
@@ -4196,17 +4476,6 @@
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="F24:I25"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:I28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -4217,11 +4486,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4241AF6E-F419-42F8-AF45-EBCD4A961F68}">
   <dimension ref="D4:K50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -4231,7 +4500,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
@@ -4245,18 +4514,18 @@
       <c r="K4" s="45"/>
     </row>
     <row r="5" spans="4:11">
-      <c r="D5" s="158" t="s">
+      <c r="D5" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="137" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="137"/>
-      <c r="J5" s="137"/>
-      <c r="K5" s="159"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="131" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="149"/>
     </row>
     <row r="6" spans="4:11" hidden="1">
       <c r="D6" s="48"/>
@@ -4269,8 +4538,8 @@
       <c r="K6" s="60"/>
     </row>
     <row r="7" spans="4:11">
-      <c r="D7" s="182"/>
-      <c r="E7" s="183"/>
+      <c r="D7" s="227"/>
+      <c r="E7" s="228"/>
       <c r="F7" s="96"/>
       <c r="G7" s="97"/>
       <c r="H7" s="98"/>
@@ -4279,15 +4548,15 @@
       <c r="K7" s="99"/>
     </row>
     <row r="8" spans="4:11">
-      <c r="D8" s="181" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="243"/>
-      <c r="F8" s="243"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
-      <c r="J8" s="125"/>
+      <c r="D8" s="215" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="206"/>
+      <c r="F8" s="206"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
       <c r="K8" s="74"/>
     </row>
     <row r="9" spans="4:11">
@@ -4301,45 +4570,45 @@
       <c r="K9" s="74"/>
     </row>
     <row r="10" spans="4:11">
-      <c r="D10" s="215" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="184" t="s">
-        <v>85</v>
-      </c>
-      <c r="H10" s="185"/>
-      <c r="I10" s="185"/>
-      <c r="J10" s="186"/>
+      <c r="D10" s="202" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="201"/>
+      <c r="F10" s="201"/>
+      <c r="G10" s="207" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="208"/>
+      <c r="I10" s="208"/>
+      <c r="J10" s="209"/>
       <c r="K10" s="76"/>
     </row>
     <row r="11" spans="4:11">
-      <c r="D11" s="191" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="175" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" s="176"/>
-      <c r="I11" s="176"/>
-      <c r="J11" s="177"/>
+      <c r="D11" s="214" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="172" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="173"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="174"/>
       <c r="K11" s="77"/>
     </row>
     <row r="12" spans="4:11">
-      <c r="D12" s="215" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="243"/>
-      <c r="F12" s="243"/>
-      <c r="G12" s="220" t="s">
-        <v>89</v>
-      </c>
-      <c r="H12" s="221"/>
-      <c r="I12" s="221"/>
-      <c r="J12" s="222"/>
+      <c r="D12" s="202" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="206"/>
+      <c r="F12" s="206"/>
+      <c r="G12" s="203" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="204"/>
+      <c r="I12" s="204"/>
+      <c r="J12" s="205"/>
       <c r="K12" s="77"/>
     </row>
     <row r="13" spans="4:11">
@@ -4353,15 +4622,15 @@
       <c r="K13" s="79"/>
     </row>
     <row r="14" spans="4:11">
-      <c r="D14" s="181" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="192"/>
-      <c r="F14" s="192"/>
-      <c r="G14" s="125"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="125"/>
-      <c r="J14" s="125"/>
+      <c r="D14" s="215" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="216"/>
+      <c r="F14" s="216"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="111"/>
       <c r="K14" s="74"/>
     </row>
     <row r="15" spans="4:11">
@@ -4373,11 +4642,11 @@
       <c r="K15" s="74"/>
     </row>
     <row r="16" spans="4:11">
-      <c r="D16" s="191" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" s="115"/>
-      <c r="F16" s="115"/>
+      <c r="D16" s="214" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="113"/>
+      <c r="F16" s="113"/>
       <c r="G16" s="81"/>
       <c r="H16" s="81"/>
       <c r="I16" s="81"/>
@@ -4395,27 +4664,27 @@
       <c r="K17" s="74"/>
     </row>
     <row r="18" spans="4:11" ht="15" customHeight="1">
-      <c r="D18" s="217" t="s">
-        <v>92</v>
-      </c>
-      <c r="E18" s="218"/>
-      <c r="F18" s="219"/>
-      <c r="G18" s="193" t="s">
-        <v>93</v>
-      </c>
-      <c r="H18" s="194"/>
-      <c r="I18" s="194"/>
-      <c r="J18" s="195"/>
+      <c r="D18" s="186" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="187"/>
+      <c r="F18" s="188"/>
+      <c r="G18" s="217" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="218"/>
+      <c r="I18" s="218"/>
+      <c r="J18" s="219"/>
       <c r="K18" s="74"/>
     </row>
     <row r="19" spans="4:11">
       <c r="D19" s="84"/>
       <c r="E19" s="85"/>
       <c r="F19" s="85"/>
-      <c r="G19" s="196"/>
-      <c r="H19" s="197"/>
-      <c r="I19" s="197"/>
-      <c r="J19" s="198"/>
+      <c r="G19" s="220"/>
+      <c r="H19" s="221"/>
+      <c r="I19" s="221"/>
+      <c r="J19" s="222"/>
       <c r="K19" s="74"/>
     </row>
     <row r="20" spans="4:11">
@@ -4429,27 +4698,27 @@
       <c r="K20" s="74"/>
     </row>
     <row r="21" spans="4:11" ht="15" customHeight="1">
-      <c r="D21" s="217" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" s="218"/>
-      <c r="F21" s="219"/>
-      <c r="G21" s="199" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" s="200"/>
-      <c r="I21" s="200"/>
-      <c r="J21" s="201"/>
+      <c r="D21" s="186" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="187"/>
+      <c r="F21" s="188"/>
+      <c r="G21" s="195" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="196"/>
+      <c r="I21" s="196"/>
+      <c r="J21" s="197"/>
       <c r="K21" s="74"/>
     </row>
     <row r="22" spans="4:11">
       <c r="D22" s="84"/>
       <c r="E22" s="85"/>
       <c r="F22" s="85"/>
-      <c r="G22" s="202"/>
-      <c r="H22" s="203"/>
-      <c r="I22" s="203"/>
-      <c r="J22" s="204"/>
+      <c r="G22" s="198"/>
+      <c r="H22" s="199"/>
+      <c r="I22" s="199"/>
+      <c r="J22" s="200"/>
       <c r="K22" s="74"/>
     </row>
     <row r="23" spans="4:11">
@@ -4463,11 +4732,11 @@
       <c r="K23" s="74"/>
     </row>
     <row r="24" spans="4:11">
-      <c r="D24" s="213" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="214"/>
-      <c r="F24" s="214"/>
+      <c r="D24" s="225" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="226"/>
+      <c r="F24" s="226"/>
       <c r="G24" s="66"/>
       <c r="H24" s="66"/>
       <c r="I24" s="66"/>
@@ -4485,27 +4754,27 @@
       <c r="K25" s="74"/>
     </row>
     <row r="26" spans="4:11" ht="15" customHeight="1">
-      <c r="D26" s="217" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" s="218"/>
-      <c r="F26" s="219"/>
-      <c r="G26" s="207" t="s">
+      <c r="D26" s="186" t="s">
         <v>97</v>
       </c>
-      <c r="H26" s="208"/>
-      <c r="I26" s="208"/>
-      <c r="J26" s="209"/>
+      <c r="E26" s="187"/>
+      <c r="F26" s="188"/>
+      <c r="G26" s="189" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" s="190"/>
+      <c r="I26" s="190"/>
+      <c r="J26" s="191"/>
       <c r="K26" s="74"/>
     </row>
     <row r="27" spans="4:11">
       <c r="D27" s="84"/>
       <c r="E27" s="85"/>
       <c r="F27" s="85"/>
-      <c r="G27" s="210"/>
-      <c r="H27" s="211"/>
-      <c r="I27" s="211"/>
-      <c r="J27" s="212"/>
+      <c r="G27" s="192"/>
+      <c r="H27" s="193"/>
+      <c r="I27" s="193"/>
+      <c r="J27" s="194"/>
       <c r="K27" s="74"/>
     </row>
     <row r="28" spans="4:11">
@@ -4520,26 +4789,26 @@
     </row>
     <row r="29" spans="4:11">
       <c r="D29" s="84"/>
-      <c r="E29" s="218" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="218"/>
-      <c r="G29" s="199" t="s">
-        <v>98</v>
-      </c>
-      <c r="H29" s="200"/>
-      <c r="I29" s="200"/>
-      <c r="J29" s="201"/>
+      <c r="E29" s="187" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="187"/>
+      <c r="G29" s="195" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="196"/>
+      <c r="I29" s="196"/>
+      <c r="J29" s="197"/>
       <c r="K29" s="74"/>
     </row>
     <row r="30" spans="4:11">
       <c r="D30" s="84"/>
       <c r="E30" s="83"/>
       <c r="F30" s="83"/>
-      <c r="G30" s="202"/>
-      <c r="H30" s="203"/>
-      <c r="I30" s="203"/>
-      <c r="J30" s="204"/>
+      <c r="G30" s="198"/>
+      <c r="H30" s="199"/>
+      <c r="I30" s="199"/>
+      <c r="J30" s="200"/>
       <c r="K30" s="74"/>
     </row>
     <row r="31" spans="4:11">
@@ -4553,11 +4822,11 @@
       <c r="K31" s="74"/>
     </row>
     <row r="32" spans="4:11">
-      <c r="D32" s="205" t="s">
-        <v>99</v>
-      </c>
-      <c r="E32" s="206"/>
-      <c r="F32" s="206"/>
+      <c r="D32" s="223" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="224"/>
+      <c r="F32" s="224"/>
       <c r="G32" s="66"/>
       <c r="H32" s="66"/>
       <c r="I32" s="66"/>
@@ -4575,27 +4844,27 @@
       <c r="K33" s="74"/>
     </row>
     <row r="34" spans="4:11" ht="15" customHeight="1">
-      <c r="D34" s="217" t="s">
-        <v>92</v>
-      </c>
-      <c r="E34" s="218"/>
-      <c r="F34" s="219"/>
-      <c r="G34" s="207" t="s">
-        <v>100</v>
-      </c>
-      <c r="H34" s="208"/>
-      <c r="I34" s="208"/>
-      <c r="J34" s="209"/>
+      <c r="D34" s="186" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="187"/>
+      <c r="F34" s="188"/>
+      <c r="G34" s="189" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="190"/>
+      <c r="I34" s="190"/>
+      <c r="J34" s="191"/>
       <c r="K34" s="74"/>
     </row>
     <row r="35" spans="4:11">
       <c r="D35" s="84"/>
       <c r="E35" s="83"/>
       <c r="F35" s="83"/>
-      <c r="G35" s="210"/>
-      <c r="H35" s="211"/>
-      <c r="I35" s="211"/>
-      <c r="J35" s="212"/>
+      <c r="G35" s="192"/>
+      <c r="H35" s="193"/>
+      <c r="I35" s="193"/>
+      <c r="J35" s="194"/>
       <c r="K35" s="74"/>
     </row>
     <row r="36" spans="4:11">
@@ -4609,27 +4878,27 @@
       <c r="K36" s="74"/>
     </row>
     <row r="37" spans="4:11" ht="15" customHeight="1">
-      <c r="D37" s="217" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="218"/>
-      <c r="F37" s="219"/>
-      <c r="G37" s="199" t="s">
-        <v>101</v>
-      </c>
-      <c r="H37" s="200"/>
-      <c r="I37" s="200"/>
-      <c r="J37" s="201"/>
+      <c r="D37" s="186" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="187"/>
+      <c r="F37" s="188"/>
+      <c r="G37" s="195" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" s="196"/>
+      <c r="I37" s="196"/>
+      <c r="J37" s="197"/>
       <c r="K37" s="74"/>
     </row>
     <row r="38" spans="4:11">
       <c r="D38" s="84"/>
       <c r="E38" s="83"/>
       <c r="F38" s="83"/>
-      <c r="G38" s="202"/>
-      <c r="H38" s="203"/>
-      <c r="I38" s="203"/>
-      <c r="J38" s="204"/>
+      <c r="G38" s="198"/>
+      <c r="H38" s="199"/>
+      <c r="I38" s="199"/>
+      <c r="J38" s="200"/>
       <c r="K38" s="74"/>
     </row>
     <row r="39" spans="4:11">
@@ -4652,7 +4921,7 @@
     </row>
     <row r="41" spans="4:11">
       <c r="D41" s="94" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E41" s="70"/>
       <c r="F41" s="69"/>
@@ -4672,16 +4941,16 @@
     </row>
     <row r="43" spans="4:11">
       <c r="D43" s="80"/>
-      <c r="E43" s="216" t="s">
-        <v>103</v>
-      </c>
-      <c r="F43" s="216"/>
-      <c r="G43" s="149" t="s">
-        <v>104</v>
-      </c>
-      <c r="H43" s="150"/>
-      <c r="I43" s="150"/>
-      <c r="J43" s="151"/>
+      <c r="E43" s="201" t="s">
+        <v>108</v>
+      </c>
+      <c r="F43" s="201"/>
+      <c r="G43" s="159" t="s">
+        <v>109</v>
+      </c>
+      <c r="H43" s="160"/>
+      <c r="I43" s="160"/>
+      <c r="J43" s="161"/>
       <c r="K43" s="74"/>
     </row>
     <row r="44" spans="4:11">
@@ -4694,16 +4963,16 @@
     </row>
     <row r="45" spans="4:11">
       <c r="D45" s="80"/>
-      <c r="E45" s="216" t="s">
-        <v>105</v>
-      </c>
-      <c r="F45" s="216"/>
-      <c r="G45" s="149" t="s">
-        <v>106</v>
-      </c>
-      <c r="H45" s="150"/>
-      <c r="I45" s="150"/>
-      <c r="J45" s="151"/>
+      <c r="E45" s="201" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45" s="201"/>
+      <c r="G45" s="159" t="s">
+        <v>111</v>
+      </c>
+      <c r="H45" s="160"/>
+      <c r="I45" s="160"/>
+      <c r="J45" s="161"/>
       <c r="K45" s="74"/>
     </row>
     <row r="46" spans="4:11">
@@ -4716,17 +4985,17 @@
       <c r="K46" s="74"/>
     </row>
     <row r="47" spans="4:11">
-      <c r="D47" s="215" t="s">
-        <v>107</v>
-      </c>
-      <c r="E47" s="216"/>
-      <c r="F47" s="216"/>
-      <c r="G47" s="149" t="s">
-        <v>108</v>
-      </c>
-      <c r="H47" s="150"/>
-      <c r="I47" s="150"/>
-      <c r="J47" s="151"/>
+      <c r="D47" s="202" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="201"/>
+      <c r="F47" s="201"/>
+      <c r="G47" s="159" t="s">
+        <v>113</v>
+      </c>
+      <c r="H47" s="160"/>
+      <c r="I47" s="160"/>
+      <c r="J47" s="161"/>
       <c r="K47" s="74"/>
     </row>
     <row r="48" spans="4:11">
@@ -4749,36 +5018,26 @@
       <c r="K49" s="103"/>
     </row>
     <row r="50" spans="4:11">
-      <c r="D50" s="187" t="s">
-        <v>109</v>
-      </c>
-      <c r="E50" s="188"/>
-      <c r="F50" s="188"/>
-      <c r="G50" s="188"/>
-      <c r="H50" s="188"/>
-      <c r="I50" s="188"/>
-      <c r="J50" s="189" t="s">
+      <c r="D50" s="210" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="211"/>
+      <c r="F50" s="211"/>
+      <c r="G50" s="211"/>
+      <c r="H50" s="211"/>
+      <c r="I50" s="211"/>
+      <c r="J50" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="K50" s="190"/>
+      <c r="K50" s="213"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="G34:J35"/>
-    <mergeCell ref="G37:J38"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="G43:J43"/>
-    <mergeCell ref="G45:J45"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="G10:J10"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="D50:I50"/>
@@ -4795,11 +5054,21 @@
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="G45:J45"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="G34:J35"/>
+    <mergeCell ref="G37:J38"/>
+    <mergeCell ref="E43:F43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4813,7 +5082,7 @@
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -4823,7 +5092,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
@@ -4837,22 +5106,22 @@
       <c r="K5" s="45"/>
     </row>
     <row r="6" spans="4:11">
-      <c r="D6" s="230" t="s">
+      <c r="D6" s="236" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="231"/>
-      <c r="F6" s="231"/>
-      <c r="G6" s="231"/>
-      <c r="H6" s="232" t="s">
-        <v>82</v>
-      </c>
-      <c r="I6" s="232"/>
-      <c r="J6" s="232"/>
-      <c r="K6" s="233"/>
+      <c r="E6" s="237"/>
+      <c r="F6" s="237"/>
+      <c r="G6" s="237"/>
+      <c r="H6" s="238" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="238"/>
+      <c r="J6" s="238"/>
+      <c r="K6" s="239"/>
     </row>
     <row r="7" spans="4:11">
-      <c r="D7" s="182"/>
-      <c r="E7" s="183"/>
+      <c r="D7" s="227"/>
+      <c r="E7" s="228"/>
       <c r="F7" s="72"/>
       <c r="G7" s="72"/>
       <c r="H7" s="72"/>
@@ -4861,15 +5130,15 @@
       <c r="K7" s="73"/>
     </row>
     <row r="8" spans="4:11">
-      <c r="D8" s="181" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="243"/>
-      <c r="F8" s="243"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
-      <c r="J8" s="125"/>
+      <c r="D8" s="215" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="206"/>
+      <c r="F8" s="206"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
       <c r="K8" s="74"/>
     </row>
     <row r="9" spans="4:11">
@@ -4883,45 +5152,45 @@
       <c r="K9" s="74"/>
     </row>
     <row r="10" spans="4:11">
-      <c r="D10" s="215" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="184" t="s">
-        <v>112</v>
-      </c>
-      <c r="H10" s="185"/>
-      <c r="I10" s="185"/>
-      <c r="J10" s="186"/>
+      <c r="D10" s="202" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="201"/>
+      <c r="F10" s="201"/>
+      <c r="G10" s="207" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" s="208"/>
+      <c r="I10" s="208"/>
+      <c r="J10" s="209"/>
       <c r="K10" s="76"/>
     </row>
     <row r="11" spans="4:11">
-      <c r="D11" s="191" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="175" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" s="176"/>
-      <c r="I11" s="176"/>
-      <c r="J11" s="177"/>
+      <c r="D11" s="214" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="172" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="173"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="174"/>
       <c r="K11" s="77"/>
     </row>
     <row r="12" spans="4:11">
-      <c r="D12" s="215" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="243"/>
-      <c r="F12" s="243"/>
-      <c r="G12" s="220" t="s">
+      <c r="D12" s="202" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="206"/>
+      <c r="F12" s="206"/>
+      <c r="G12" s="203" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="221"/>
-      <c r="I12" s="221"/>
-      <c r="J12" s="222"/>
+      <c r="H12" s="204"/>
+      <c r="I12" s="204"/>
+      <c r="J12" s="205"/>
       <c r="K12" s="77"/>
     </row>
     <row r="13" spans="4:11">
@@ -4935,15 +5204,15 @@
       <c r="K13" s="79"/>
     </row>
     <row r="14" spans="4:11">
-      <c r="D14" s="223" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" s="115"/>
-      <c r="F14" s="115"/>
-      <c r="G14" s="125"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="125"/>
-      <c r="J14" s="125"/>
+      <c r="D14" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="111"/>
       <c r="K14" s="74"/>
     </row>
     <row r="15" spans="4:11">
@@ -4955,27 +5224,27 @@
       <c r="K15" s="74"/>
     </row>
     <row r="16" spans="4:11" ht="15" customHeight="1">
-      <c r="D16" s="217" t="s">
-        <v>114</v>
-      </c>
-      <c r="E16" s="218"/>
-      <c r="F16" s="219"/>
-      <c r="G16" s="193" t="s">
-        <v>115</v>
-      </c>
-      <c r="H16" s="224"/>
-      <c r="I16" s="224"/>
-      <c r="J16" s="225"/>
+      <c r="D16" s="186" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" s="187"/>
+      <c r="F16" s="188"/>
+      <c r="G16" s="217" t="s">
+        <v>120</v>
+      </c>
+      <c r="H16" s="231"/>
+      <c r="I16" s="231"/>
+      <c r="J16" s="232"/>
       <c r="K16" s="74"/>
     </row>
     <row r="17" spans="4:11">
       <c r="D17" s="82"/>
       <c r="E17" s="83"/>
       <c r="F17" s="83"/>
-      <c r="G17" s="226"/>
-      <c r="H17" s="227"/>
-      <c r="I17" s="227"/>
-      <c r="J17" s="228"/>
+      <c r="G17" s="233"/>
+      <c r="H17" s="234"/>
+      <c r="I17" s="234"/>
+      <c r="J17" s="235"/>
       <c r="K17" s="74"/>
     </row>
     <row r="18" spans="4:11">
@@ -5000,10 +5269,10 @@
     </row>
     <row r="20" spans="4:11" s="92" customFormat="1">
       <c r="D20" s="229" t="s">
-        <v>116</v>
-      </c>
-      <c r="E20" s="206"/>
-      <c r="F20" s="206"/>
+        <v>121</v>
+      </c>
+      <c r="E20" s="224"/>
+      <c r="F20" s="224"/>
       <c r="G20" s="66"/>
       <c r="H20" s="66"/>
       <c r="I20" s="66"/>
@@ -5023,33 +5292,33 @@
     <row r="22" spans="4:11">
       <c r="D22" s="87"/>
       <c r="E22" s="71"/>
-      <c r="F22" s="207" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22" s="208"/>
-      <c r="H22" s="208"/>
-      <c r="I22" s="208"/>
-      <c r="J22" s="209"/>
+      <c r="F22" s="189" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="190"/>
+      <c r="H22" s="190"/>
+      <c r="I22" s="190"/>
+      <c r="J22" s="191"/>
       <c r="K22" s="74"/>
     </row>
     <row r="23" spans="4:11">
       <c r="D23" s="82"/>
       <c r="E23" s="83"/>
-      <c r="F23" s="210"/>
-      <c r="G23" s="211"/>
-      <c r="H23" s="211"/>
-      <c r="I23" s="211"/>
-      <c r="J23" s="212"/>
+      <c r="F23" s="192"/>
+      <c r="G23" s="193"/>
+      <c r="H23" s="193"/>
+      <c r="I23" s="193"/>
+      <c r="J23" s="194"/>
       <c r="K23" s="74"/>
     </row>
     <row r="24" spans="4:11">
       <c r="D24" s="82"/>
       <c r="E24" s="83"/>
       <c r="F24" s="83"/>
-      <c r="G24" s="242"/>
-      <c r="H24" s="242"/>
-      <c r="I24" s="242"/>
-      <c r="J24" s="242"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
       <c r="K24" s="74"/>
     </row>
     <row r="25" spans="4:11">
@@ -5063,22 +5332,33 @@
       <c r="K25" s="91"/>
     </row>
     <row r="26" spans="4:11">
-      <c r="D26" s="187" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" s="188"/>
-      <c r="F26" s="188"/>
-      <c r="G26" s="188"/>
-      <c r="H26" s="188"/>
-      <c r="I26" s="188"/>
-      <c r="J26" s="189" t="s">
+      <c r="D26" s="210" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="211"/>
+      <c r="F26" s="211"/>
+      <c r="G26" s="211"/>
+      <c r="H26" s="211"/>
+      <c r="I26" s="211"/>
+      <c r="J26" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="K26" s="190"/>
+      <c r="K26" s="213"/>
     </row>
     <row r="35" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:J12"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D26:I26"/>
     <mergeCell ref="J26:K26"/>
@@ -5087,17 +5367,6 @@
     <mergeCell ref="G14:J14"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="G16:J17"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5107,11 +5376,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46F92D6-0887-4A5A-AFC7-87E289EC819A}">
   <dimension ref="D4:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -5121,7 +5390,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
@@ -5135,22 +5404,22 @@
       <c r="K4" s="45"/>
     </row>
     <row r="5" spans="4:11">
-      <c r="D5" s="230" t="s">
+      <c r="D5" s="236" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="231"/>
-      <c r="F5" s="231"/>
-      <c r="G5" s="231"/>
-      <c r="H5" s="232" t="s">
-        <v>110</v>
-      </c>
-      <c r="I5" s="232"/>
-      <c r="J5" s="232"/>
-      <c r="K5" s="233"/>
+      <c r="E5" s="237"/>
+      <c r="F5" s="237"/>
+      <c r="G5" s="237"/>
+      <c r="H5" s="238" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" s="238"/>
+      <c r="J5" s="238"/>
+      <c r="K5" s="239"/>
     </row>
     <row r="6" spans="4:11">
-      <c r="D6" s="182"/>
-      <c r="E6" s="183"/>
+      <c r="D6" s="227"/>
+      <c r="E6" s="228"/>
       <c r="F6" s="72"/>
       <c r="G6" s="72"/>
       <c r="H6" s="72"/>
@@ -5159,15 +5428,15 @@
       <c r="K6" s="73"/>
     </row>
     <row r="7" spans="4:11">
-      <c r="D7" s="181" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" s="243"/>
-      <c r="F7" s="243"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
-      <c r="J7" s="125"/>
+      <c r="D7" s="215" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="206"/>
+      <c r="F7" s="206"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
       <c r="K7" s="74"/>
     </row>
     <row r="8" spans="4:11">
@@ -5181,45 +5450,45 @@
       <c r="K8" s="74"/>
     </row>
     <row r="9" spans="4:11">
-      <c r="D9" s="215" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="216"/>
-      <c r="F9" s="216"/>
-      <c r="G9" s="184" t="s">
-        <v>121</v>
-      </c>
-      <c r="H9" s="185"/>
-      <c r="I9" s="185"/>
-      <c r="J9" s="186"/>
+      <c r="D9" s="202" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="201"/>
+      <c r="F9" s="201"/>
+      <c r="G9" s="207" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="208"/>
+      <c r="I9" s="208"/>
+      <c r="J9" s="209"/>
       <c r="K9" s="76"/>
     </row>
     <row r="10" spans="4:11">
-      <c r="D10" s="191" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
-      <c r="G10" s="175" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="176"/>
-      <c r="I10" s="176"/>
-      <c r="J10" s="177"/>
+      <c r="D10" s="214" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="172" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="173"/>
+      <c r="I10" s="173"/>
+      <c r="J10" s="174"/>
       <c r="K10" s="77"/>
     </row>
     <row r="11" spans="4:11">
-      <c r="D11" s="215" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="243"/>
-      <c r="F11" s="243"/>
-      <c r="G11" s="220" t="s">
-        <v>122</v>
-      </c>
-      <c r="H11" s="221"/>
-      <c r="I11" s="221"/>
-      <c r="J11" s="222"/>
+      <c r="D11" s="202" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="206"/>
+      <c r="F11" s="206"/>
+      <c r="G11" s="203" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" s="204"/>
+      <c r="I11" s="204"/>
+      <c r="J11" s="205"/>
       <c r="K11" s="77"/>
     </row>
     <row r="12" spans="4:11">
@@ -5233,15 +5502,15 @@
       <c r="K12" s="79"/>
     </row>
     <row r="13" spans="4:11">
-      <c r="D13" s="223" t="s">
-        <v>123</v>
-      </c>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="125"/>
-      <c r="H13" s="125"/>
-      <c r="I13" s="125"/>
-      <c r="J13" s="125"/>
+      <c r="D13" s="230" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
       <c r="K13" s="74"/>
     </row>
     <row r="14" spans="4:11">
@@ -5253,27 +5522,27 @@
       <c r="K14" s="74"/>
     </row>
     <row r="15" spans="4:11" ht="15" customHeight="1">
-      <c r="D15" s="217" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" s="218"/>
-      <c r="F15" s="219"/>
-      <c r="G15" s="193" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" s="224"/>
-      <c r="I15" s="224"/>
-      <c r="J15" s="225"/>
+      <c r="D15" s="186" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="187"/>
+      <c r="F15" s="188"/>
+      <c r="G15" s="217" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" s="231"/>
+      <c r="I15" s="231"/>
+      <c r="J15" s="232"/>
       <c r="K15" s="74"/>
     </row>
     <row r="16" spans="4:11">
       <c r="D16" s="82"/>
       <c r="E16" s="83"/>
       <c r="F16" s="83"/>
-      <c r="G16" s="226"/>
-      <c r="H16" s="227"/>
-      <c r="I16" s="227"/>
-      <c r="J16" s="228"/>
+      <c r="G16" s="233"/>
+      <c r="H16" s="234"/>
+      <c r="I16" s="234"/>
+      <c r="J16" s="235"/>
       <c r="K16" s="74"/>
     </row>
     <row r="17" spans="4:11">
@@ -5287,27 +5556,27 @@
       <c r="K17" s="74"/>
     </row>
     <row r="18" spans="4:11" ht="15" customHeight="1">
-      <c r="D18" s="217" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="218"/>
-      <c r="F18" s="219"/>
-      <c r="G18" s="193" t="s">
-        <v>127</v>
-      </c>
-      <c r="H18" s="224"/>
-      <c r="I18" s="224"/>
-      <c r="J18" s="225"/>
+      <c r="D18" s="186" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="187"/>
+      <c r="F18" s="188"/>
+      <c r="G18" s="217" t="s">
+        <v>132</v>
+      </c>
+      <c r="H18" s="231"/>
+      <c r="I18" s="231"/>
+      <c r="J18" s="232"/>
       <c r="K18" s="74"/>
     </row>
     <row r="19" spans="4:11">
       <c r="D19" s="82"/>
       <c r="E19" s="83"/>
       <c r="F19" s="83"/>
-      <c r="G19" s="226"/>
-      <c r="H19" s="227"/>
-      <c r="I19" s="227"/>
-      <c r="J19" s="228"/>
+      <c r="G19" s="233"/>
+      <c r="H19" s="234"/>
+      <c r="I19" s="234"/>
+      <c r="J19" s="235"/>
       <c r="K19" s="74"/>
     </row>
     <row r="20" spans="4:11">
@@ -5331,11 +5600,11 @@
       <c r="K21" s="93"/>
     </row>
     <row r="22" spans="4:11" ht="15" customHeight="1">
-      <c r="D22" s="234" t="s">
-        <v>128</v>
-      </c>
-      <c r="E22" s="218"/>
-      <c r="F22" s="218"/>
+      <c r="D22" s="240" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="187"/>
+      <c r="F22" s="187"/>
       <c r="G22" s="71"/>
       <c r="H22" s="81"/>
       <c r="I22" s="81"/>
@@ -5353,27 +5622,27 @@
       <c r="K23" s="74"/>
     </row>
     <row r="24" spans="4:11" ht="15" customHeight="1">
-      <c r="D24" s="238" t="s">
-        <v>129</v>
-      </c>
-      <c r="E24" s="218"/>
-      <c r="F24" s="219"/>
-      <c r="G24" s="207" t="s">
-        <v>130</v>
-      </c>
-      <c r="H24" s="208"/>
-      <c r="I24" s="208"/>
-      <c r="J24" s="209"/>
+      <c r="D24" s="244" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" s="187"/>
+      <c r="F24" s="188"/>
+      <c r="G24" s="189" t="s">
+        <v>135</v>
+      </c>
+      <c r="H24" s="190"/>
+      <c r="I24" s="190"/>
+      <c r="J24" s="191"/>
       <c r="K24" s="74"/>
     </row>
     <row r="25" spans="4:11">
       <c r="D25" s="82"/>
       <c r="E25" s="83"/>
       <c r="F25" s="83"/>
-      <c r="G25" s="210"/>
-      <c r="H25" s="211"/>
-      <c r="I25" s="211"/>
-      <c r="J25" s="212"/>
+      <c r="G25" s="192"/>
+      <c r="H25" s="193"/>
+      <c r="I25" s="193"/>
+      <c r="J25" s="194"/>
       <c r="K25" s="74"/>
     </row>
     <row r="26" spans="4:11">
@@ -5387,27 +5656,27 @@
       <c r="K26" s="74"/>
     </row>
     <row r="27" spans="4:11" ht="15.75">
-      <c r="D27" s="235" t="s">
-        <v>131</v>
-      </c>
-      <c r="E27" s="236"/>
-      <c r="F27" s="237"/>
-      <c r="G27" s="207" t="s">
-        <v>132</v>
-      </c>
-      <c r="H27" s="208"/>
-      <c r="I27" s="208"/>
-      <c r="J27" s="209"/>
+      <c r="D27" s="241" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="242"/>
+      <c r="F27" s="243"/>
+      <c r="G27" s="189" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" s="190"/>
+      <c r="I27" s="190"/>
+      <c r="J27" s="191"/>
       <c r="K27" s="74"/>
     </row>
     <row r="28" spans="4:11">
       <c r="D28" s="82"/>
       <c r="E28" s="83"/>
       <c r="F28" s="83"/>
-      <c r="G28" s="210"/>
-      <c r="H28" s="211"/>
-      <c r="I28" s="211"/>
-      <c r="J28" s="212"/>
+      <c r="G28" s="192"/>
+      <c r="H28" s="193"/>
+      <c r="I28" s="193"/>
+      <c r="J28" s="194"/>
       <c r="K28" s="74"/>
     </row>
     <row r="29" spans="4:11">
@@ -5421,35 +5690,21 @@
       <c r="K29" s="91"/>
     </row>
     <row r="30" spans="4:11">
-      <c r="D30" s="187" t="s">
-        <v>133</v>
-      </c>
-      <c r="E30" s="188"/>
-      <c r="F30" s="188"/>
-      <c r="G30" s="188"/>
-      <c r="H30" s="188"/>
-      <c r="I30" s="188"/>
-      <c r="J30" s="189" t="s">
+      <c r="D30" s="210" t="s">
+        <v>138</v>
+      </c>
+      <c r="E30" s="211"/>
+      <c r="F30" s="211"/>
+      <c r="G30" s="211"/>
+      <c r="H30" s="211"/>
+      <c r="I30" s="211"/>
+      <c r="J30" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="K30" s="190"/>
+      <c r="K30" s="213"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:J19"/>
-    <mergeCell ref="D30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="G27:J28"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G24:J25"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="D15:F15"/>
@@ -5460,6 +5715,20 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G15:J16"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:J19"/>
+    <mergeCell ref="D30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="G27:J28"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G24:J25"/>
+    <mergeCell ref="D24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5473,17 +5742,17 @@
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="3:13" ht="15.75" thickBot="1"/>
     <row r="3" spans="3:13">
       <c r="C3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="239" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" s="239"/>
+      <c r="D3" s="245" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="245"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="28" t="s">
@@ -5495,24 +5764,24 @@
       <c r="J3" s="30"/>
     </row>
     <row r="4" spans="3:13">
-      <c r="C4" s="240" t="s">
+      <c r="C4" s="246" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="231"/>
-      <c r="E4" s="231"/>
-      <c r="F4" s="231"/>
-      <c r="G4" s="232" t="s">
-        <v>135</v>
-      </c>
-      <c r="H4" s="232"/>
-      <c r="I4" s="232"/>
-      <c r="J4" s="241"/>
+      <c r="D4" s="237"/>
+      <c r="E4" s="237"/>
+      <c r="F4" s="237"/>
+      <c r="G4" s="238" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" s="238"/>
+      <c r="I4" s="238"/>
+      <c r="J4" s="247"/>
     </row>
     <row r="5" spans="3:13">
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="113"/>
+      <c r="D5" s="115"/>
       <c r="J5" s="14"/>
     </row>
     <row r="6" spans="3:13">
@@ -5520,31 +5789,31 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="3:13">
-      <c r="C7" s="114" t="s">
+      <c r="C7" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="125" t="s">
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="3:13">
-      <c r="C8" s="114" t="s">
+      <c r="C8" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="115"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="125" t="s">
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="3:13">
@@ -5558,11 +5827,11 @@
       <c r="J9" s="17"/>
     </row>
     <row r="10" spans="3:13">
-      <c r="C10" s="112" t="s">
-        <v>136</v>
-      </c>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
+      <c r="C10" s="114" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="115"/>
+      <c r="E10" s="115"/>
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="3:13">
@@ -5570,45 +5839,45 @@
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="3:13">
-      <c r="C12" s="114" t="s">
+      <c r="C12" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="115"/>
-      <c r="E12" s="115"/>
-      <c r="F12" s="125" t="s">
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="125"/>
-      <c r="H12" s="125"/>
-      <c r="I12" s="125"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="111"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="3:13">
-      <c r="C13" s="114" t="s">
+      <c r="C13" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="125" t="s">
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="125"/>
-      <c r="H13" s="125"/>
-      <c r="I13" s="125"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="3:13">
-      <c r="C14" s="114" t="s">
+      <c r="C14" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="115"/>
-      <c r="E14" s="115"/>
-      <c r="F14" s="125" t="s">
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="125"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="125"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="111"/>
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="3:13" ht="15.75">
@@ -5623,10 +5892,10 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="3:13">
-      <c r="C16" s="112" t="s">
-        <v>137</v>
-      </c>
-      <c r="D16" s="113"/>
+      <c r="C16" s="114" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="115"/>
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="3:16">
@@ -5634,17 +5903,17 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="3:16">
-      <c r="C18" s="114" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" s="115"/>
-      <c r="E18" s="115"/>
-      <c r="F18" s="125" t="s">
-        <v>139</v>
-      </c>
-      <c r="G18" s="125"/>
-      <c r="H18" s="125"/>
-      <c r="I18" s="125"/>
+      <c r="C18" s="112" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="111" t="s">
+        <v>144</v>
+      </c>
+      <c r="G18" s="111"/>
+      <c r="H18" s="111"/>
+      <c r="I18" s="111"/>
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="3:16" ht="15" customHeight="1">
@@ -5658,17 +5927,17 @@
       <c r="J19" s="106"/>
     </row>
     <row r="20" spans="3:16">
-      <c r="C20" s="114" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="115"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="125" t="s">
-        <v>141</v>
-      </c>
-      <c r="G20" s="125"/>
-      <c r="H20" s="125"/>
-      <c r="I20" s="125"/>
+      <c r="C20" s="112" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="113"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="111" t="s">
+        <v>146</v>
+      </c>
+      <c r="G20" s="111"/>
+      <c r="H20" s="111"/>
+      <c r="I20" s="111"/>
       <c r="J20" s="106"/>
     </row>
     <row r="21" spans="3:16">
@@ -5676,85 +5945,85 @@
       <c r="J21" s="14"/>
     </row>
     <row r="22" spans="3:16">
-      <c r="C22" s="114" t="s">
-        <v>142</v>
-      </c>
-      <c r="D22" s="115"/>
-      <c r="E22" s="115"/>
+      <c r="C22" s="112" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="113"/>
+      <c r="E22" s="113"/>
       <c r="J22" s="14"/>
     </row>
     <row r="23" spans="3:16" ht="15" customHeight="1">
       <c r="C23" s="13"/>
-      <c r="D23" s="126" t="s">
-        <v>143</v>
-      </c>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
-      <c r="G23" s="127"/>
-      <c r="H23" s="127"/>
-      <c r="I23" s="127"/>
-      <c r="J23" s="128"/>
+      <c r="D23" s="133" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="134"/>
+      <c r="F23" s="134"/>
+      <c r="G23" s="134"/>
+      <c r="H23" s="134"/>
+      <c r="I23" s="134"/>
+      <c r="J23" s="135"/>
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="3:16">
       <c r="C24" s="13"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="130"/>
-      <c r="F24" s="130"/>
-      <c r="G24" s="130"/>
-      <c r="H24" s="130"/>
-      <c r="I24" s="130"/>
-      <c r="J24" s="131"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="137"/>
+      <c r="G24" s="137"/>
+      <c r="H24" s="137"/>
+      <c r="I24" s="137"/>
+      <c r="J24" s="138"/>
     </row>
     <row r="25" spans="3:16">
       <c r="C25" s="13"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="130"/>
-      <c r="F25" s="130"/>
-      <c r="G25" s="130"/>
-      <c r="H25" s="130"/>
-      <c r="I25" s="130"/>
-      <c r="J25" s="131"/>
+      <c r="D25" s="136"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="137"/>
+      <c r="G25" s="137"/>
+      <c r="H25" s="137"/>
+      <c r="I25" s="137"/>
+      <c r="J25" s="138"/>
     </row>
     <row r="26" spans="3:16">
       <c r="C26" s="13"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="130"/>
-      <c r="G26" s="130"/>
-      <c r="H26" s="130"/>
-      <c r="I26" s="130"/>
-      <c r="J26" s="131"/>
+      <c r="D26" s="136"/>
+      <c r="E26" s="137"/>
+      <c r="F26" s="137"/>
+      <c r="G26" s="137"/>
+      <c r="H26" s="137"/>
+      <c r="I26" s="137"/>
+      <c r="J26" s="138"/>
     </row>
     <row r="27" spans="3:16">
       <c r="C27" s="13"/>
-      <c r="D27" s="129"/>
-      <c r="E27" s="130"/>
-      <c r="F27" s="130"/>
-      <c r="G27" s="130"/>
-      <c r="H27" s="130"/>
-      <c r="I27" s="130"/>
-      <c r="J27" s="131"/>
+      <c r="D27" s="136"/>
+      <c r="E27" s="137"/>
+      <c r="F27" s="137"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="137"/>
+      <c r="J27" s="138"/>
     </row>
     <row r="28" spans="3:16">
       <c r="C28" s="13"/>
-      <c r="D28" s="129"/>
-      <c r="E28" s="130"/>
-      <c r="F28" s="130"/>
-      <c r="G28" s="130"/>
-      <c r="H28" s="130"/>
-      <c r="I28" s="130"/>
-      <c r="J28" s="131"/>
+      <c r="D28" s="136"/>
+      <c r="E28" s="137"/>
+      <c r="F28" s="137"/>
+      <c r="G28" s="137"/>
+      <c r="H28" s="137"/>
+      <c r="I28" s="137"/>
+      <c r="J28" s="138"/>
     </row>
     <row r="29" spans="3:16">
       <c r="C29" s="13"/>
-      <c r="D29" s="132"/>
-      <c r="E29" s="133"/>
-      <c r="F29" s="133"/>
-      <c r="G29" s="133"/>
-      <c r="H29" s="133"/>
-      <c r="I29" s="133"/>
-      <c r="J29" s="134"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="140"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="140"/>
+      <c r="I29" s="140"/>
+      <c r="J29" s="141"/>
     </row>
     <row r="30" spans="3:16">
       <c r="C30" s="13"/>
@@ -5777,21 +6046,32 @@
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="3:16" ht="15.75" thickBot="1">
-      <c r="C32" s="108" t="s">
-        <v>144</v>
-      </c>
-      <c r="D32" s="109"/>
-      <c r="E32" s="109"/>
-      <c r="F32" s="109"/>
-      <c r="G32" s="109"/>
-      <c r="H32" s="109"/>
-      <c r="I32" s="110" t="s">
+      <c r="C32" s="116" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="117"/>
+      <c r="E32" s="117"/>
+      <c r="F32" s="117"/>
+      <c r="G32" s="117"/>
+      <c r="H32" s="117"/>
+      <c r="I32" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="J32" s="111"/>
+      <c r="J32" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:I13"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D23:J29"/>
     <mergeCell ref="C8:E8"/>
@@ -5805,17 +6085,6 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:I7"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>